<commit_message>
this contains the notes for the spi-ethercat first tests
</commit_message>
<xml_diff>
--- a/Admin/Arbeitszeiterfassung-2020-jcr.xlsx
+++ b/Admin/Arbeitszeiterfassung-2020-jcr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Projektarbeit\Admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Projektarbeit_Docs\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22A9DC6-6877-4C1D-B2DA-2D1B2916865D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633ACE76-105D-4CF7-9985-795B2ACFA4D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Voreinstellungen" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="170">
   <si>
     <t>Benutzer-Voreinstellungen</t>
   </si>
@@ -647,6 +647,18 @@
   </si>
   <si>
     <t>Library OK-Placing Parts+Keys=Delayed</t>
+  </si>
+  <si>
+    <t>SPI Theory = Delayed Result</t>
+  </si>
+  <si>
+    <t>PCB Change all elements = Delayed Results</t>
+  </si>
+  <si>
+    <t>PCB Bad Routing+GIT Problems=No Results</t>
+  </si>
+  <si>
+    <t>PCB Aligned-Final Routing=Results!</t>
   </si>
 </sst>
 </file>
@@ -7029,6 +7041,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9CE840A-BD0A-4D27-AF95-2193919D69FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5294164-5D5E-42FD-87C8-7E1A44422969}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7929,6 +8049,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8906287-F7E2-4AE8-B456-052B901F25CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FA3A69E-CAEC-424B-8124-C73781CE8F8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8894,7 +9122,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-6.7881944444444402</v>
+        <v>-5.6631944444444304</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8939,7 +9167,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-6.7881944444444402</v>
+        <v>-5.6631944444444304</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8984,7 +9212,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.7881944444444402</v>
+        <v>-5.6631944444444304</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9029,7 +9257,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.7881944444444402</v>
+        <v>-5.6631944444444304</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9074,7 +9302,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.1215277777777697</v>
+        <v>-5.9965277777777599</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9119,7 +9347,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.2881944444444402</v>
+        <v>-6.1631944444444304</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9164,7 +9392,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.6215277777777697</v>
+        <v>-6.4965277777777599</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9209,7 +9437,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.6215277777777697</v>
+        <v>-6.4965277777777599</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9254,7 +9482,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.6215277777777697</v>
+        <v>-6.4965277777777599</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9299,7 +9527,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.6215277777777697</v>
+        <v>-6.4965277777777599</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9344,7 +9572,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.6215277777777697</v>
+        <v>-6.4965277777777599</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9389,7 +9617,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.9548611111111001</v>
+        <v>-6.8298611111110903</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9434,7 +9662,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.1215277777777697</v>
+        <v>-6.9965277777777599</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9479,7 +9707,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.4548611111111001</v>
+        <v>-7.3298611111110903</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9524,7 +9752,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.4548611111111001</v>
+        <v>-7.3298611111110903</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9569,7 +9797,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.4548611111111001</v>
+        <v>-7.3298611111110903</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9614,7 +9842,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.4548611111111001</v>
+        <v>-7.3298611111110903</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9659,7 +9887,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.4548611111111001</v>
+        <v>-7.3298611111110903</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9704,7 +9932,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.7881944444444304</v>
+        <v>-7.6631944444444198</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9749,7 +9977,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.9548611111111001</v>
+        <v>-7.8298611111110903</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9794,7 +10022,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.2881944444444304</v>
+        <v>-8.1631944444444198</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9839,7 +10067,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.2881944444444304</v>
+        <v>-8.1631944444444198</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9884,7 +10112,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.2881944444444304</v>
+        <v>-8.1631944444444198</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9929,7 +10157,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.2881944444444304</v>
+        <v>-8.1631944444444198</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9974,7 +10202,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.2881944444444304</v>
+        <v>-8.1631944444444198</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10019,7 +10247,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.6215277777777608</v>
+        <v>-8.4965277777777501</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10064,7 +10292,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.7881944444444304</v>
+        <v>-8.6631944444444198</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10109,7 +10337,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.1215277777778</v>
+        <v>-8.9965277777777501</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10154,7 +10382,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.1215277777778</v>
+        <v>-8.9965277777777501</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10199,7 +10427,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.1215277777778</v>
+        <v>-8.9965277777777501</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10244,7 +10472,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.1215277777778</v>
+        <v>-8.9965277777777501</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -10275,7 +10503,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">Juli!F40</f>
-        <v>-6.7881944444444402</v>
+        <v>-5.6631944444444304</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -10396,7 +10624,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-10.1215277777778</v>
+        <v>-8.9965277777777608</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -10845,7 +11073,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-10.1215277777778</v>
+        <v>-8.9965277777777608</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10890,7 +11118,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-10.4548611111111</v>
+        <v>-9.3298611111110894</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10935,7 +11163,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.6215277777778</v>
+        <v>-9.4965277777777608</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10980,7 +11208,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.9548611111111</v>
+        <v>-9.8298611111110894</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11025,7 +11253,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.9548611111111</v>
+        <v>-9.8298611111110894</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11070,7 +11298,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.9548611111111</v>
+        <v>-9.8298611111110894</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11115,7 +11343,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.9548611111111</v>
+        <v>-9.8298611111110894</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11160,7 +11388,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.9548611111111</v>
+        <v>-9.8298611111110894</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11205,7 +11433,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.2881944444444</v>
+        <v>-10.1631944444444</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11250,7 +11478,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.4548611111111</v>
+        <v>-10.3298611111111</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11295,7 +11523,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.7881944444444</v>
+        <v>-10.6631944444444</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11340,7 +11568,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.7881944444444</v>
+        <v>-10.6631944444444</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11385,7 +11613,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.7881944444444</v>
+        <v>-10.6631944444444</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11430,7 +11658,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.7881944444444</v>
+        <v>-10.6631944444444</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11475,7 +11703,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.7881944444444</v>
+        <v>-10.6631944444444</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11520,7 +11748,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.1215277777777</v>
+        <v>-10.9965277777777</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11565,7 +11793,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.2881944444444</v>
+        <v>-11.1631944444444</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11610,7 +11838,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.6215277777777</v>
+        <v>-11.4965277777777</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11655,7 +11883,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.6215277777777</v>
+        <v>-11.4965277777777</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11700,7 +11928,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.6215277777777</v>
+        <v>-11.4965277777777</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11745,7 +11973,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.6215277777777</v>
+        <v>-11.4965277777777</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11790,7 +12018,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.6215277777777</v>
+        <v>-11.4965277777777</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11835,7 +12063,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.954861111111001</v>
+        <v>-11.829861111111001</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11880,7 +12108,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.1215277777777</v>
+        <v>-11.9965277777777</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11925,7 +12153,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.454861111111001</v>
+        <v>-12.329861111111001</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11970,7 +12198,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.454861111111001</v>
+        <v>-12.329861111111001</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12015,7 +12243,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.454861111111001</v>
+        <v>-12.329861111111001</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12060,7 +12288,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.454861111111001</v>
+        <v>-12.329861111111001</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12105,7 +12333,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.454861111111001</v>
+        <v>-12.329861111111001</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12150,7 +12378,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.788194444444301</v>
+        <v>-12.663194444444301</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12226,7 +12454,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">August!F40</f>
-        <v>-10.1215277777778</v>
+        <v>-8.9965277777777608</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -12347,7 +12575,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-13.7881944444445</v>
+        <v>-12.6631944444444</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -12796,7 +13024,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-13.9548611111112</v>
+        <v>-12.8298611111111</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12841,7 +13069,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-14.2881944444445</v>
+        <v>-13.1631944444444</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12886,7 +13114,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.2881944444445</v>
+        <v>-13.1631944444444</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12931,7 +13159,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.2881944444445</v>
+        <v>-13.1631944444444</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12976,7 +13204,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.2881944444445</v>
+        <v>-13.1631944444444</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13021,7 +13249,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.2881944444445</v>
+        <v>-13.1631944444444</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13066,7 +13294,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.6215277777778</v>
+        <v>-13.4965277777777</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13111,7 +13339,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.7881944444445</v>
+        <v>-13.6631944444444</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13156,7 +13384,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.1215277777778</v>
+        <v>-13.9965277777777</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13201,7 +13429,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.1215277777778</v>
+        <v>-13.9965277777777</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13246,7 +13474,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.1215277777778</v>
+        <v>-13.9965277777777</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13291,7 +13519,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.1215277777778</v>
+        <v>-13.9965277777777</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13336,7 +13564,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.1215277777778</v>
+        <v>-13.9965277777777</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13381,7 +13609,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.4548611111111</v>
+        <v>-14.329861111111001</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13426,7 +13654,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.6215277777778</v>
+        <v>-14.4965277777777</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13471,7 +13699,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.9548611111111</v>
+        <v>-14.829861111111001</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13516,7 +13744,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.9548611111111</v>
+        <v>-14.829861111111001</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13561,7 +13789,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.9548611111111</v>
+        <v>-14.829861111111001</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13606,7 +13834,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.9548611111111</v>
+        <v>-14.829861111111001</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13651,7 +13879,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.9548611111111</v>
+        <v>-14.829861111111001</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13696,7 +13924,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.2881944444444</v>
+        <v>-15.163194444444301</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13741,7 +13969,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.4548611111111</v>
+        <v>-15.329861111111001</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13786,7 +14014,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.7881944444444</v>
+        <v>-15.663194444444301</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13831,7 +14059,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.7881944444444</v>
+        <v>-15.663194444444301</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13876,7 +14104,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.7881944444444</v>
+        <v>-15.663194444444301</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13921,7 +14149,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.7881944444444</v>
+        <v>-15.663194444444301</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13966,7 +14194,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.7881944444444</v>
+        <v>-15.663194444444301</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14011,7 +14239,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.1215277777777</v>
+        <v>-15.996527777777599</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14056,7 +14284,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.2881944444444</v>
+        <v>-16.163194444444301</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14101,7 +14329,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.6215277777777</v>
+        <v>-16.496527777777601</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14146,7 +14374,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.6215277777777</v>
+        <v>-16.496527777777601</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -14177,7 +14405,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">September!F40</f>
-        <v>-13.7881944444445</v>
+        <v>-12.6631944444444</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -14298,7 +14526,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-17.6215277777778</v>
+        <v>-16.4965277777777</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -14747,7 +14975,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-17.6215277777778</v>
+        <v>-16.4965277777777</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14792,7 +15020,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-17.6215277777778</v>
+        <v>-16.4965277777777</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14837,7 +15065,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.6215277777778</v>
+        <v>-16.4965277777777</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14882,7 +15110,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.9548611111111</v>
+        <v>-16.829861111111001</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14927,7 +15155,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.1215277777778</v>
+        <v>-16.9965277777777</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14972,7 +15200,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.4548611111111</v>
+        <v>-17.329861111111001</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15017,7 +15245,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.4548611111111</v>
+        <v>-17.329861111111001</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15062,7 +15290,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.4548611111111</v>
+        <v>-17.329861111111001</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15107,7 +15335,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.4548611111111</v>
+        <v>-17.329861111111001</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15152,7 +15380,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.4548611111111</v>
+        <v>-17.329861111111001</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15197,7 +15425,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.7881944444444</v>
+        <v>-17.663194444444301</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15242,7 +15470,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.9548611111111</v>
+        <v>-17.829861111111001</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15287,7 +15515,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.2881944444444</v>
+        <v>-18.163194444444301</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15332,7 +15560,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.2881944444444</v>
+        <v>-18.163194444444301</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15377,7 +15605,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.2881944444444</v>
+        <v>-18.163194444444301</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15422,7 +15650,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.2881944444444</v>
+        <v>-18.163194444444301</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15467,7 +15695,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.2881944444444</v>
+        <v>-18.163194444444301</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15512,7 +15740,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.6215277777777</v>
+        <v>-18.496527777777601</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15557,7 +15785,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.7881944444444</v>
+        <v>-18.663194444444301</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15602,7 +15830,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.1215277777777</v>
+        <v>-18.996527777777601</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15647,7 +15875,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.1215277777777</v>
+        <v>-18.996527777777601</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15692,7 +15920,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.1215277777777</v>
+        <v>-18.996527777777601</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15737,7 +15965,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.1215277777777</v>
+        <v>-18.996527777777601</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15782,7 +16010,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.1215277777777</v>
+        <v>-18.996527777777601</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15827,7 +16055,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.454861111111001</v>
+        <v>-19.329861111110901</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15872,7 +16100,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.6215277777777</v>
+        <v>-19.496527777777601</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15917,7 +16145,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.954861111111001</v>
+        <v>-19.829861111110901</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15962,7 +16190,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.954861111111001</v>
+        <v>-19.829861111110901</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16007,7 +16235,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.954861111111001</v>
+        <v>-19.829861111110901</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16052,7 +16280,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.954861111111001</v>
+        <v>-19.829861111110901</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16128,7 +16356,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">Oktober!F40</f>
-        <v>-17.6215277777778</v>
+        <v>-16.4965277777777</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -16249,7 +16477,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-20.9548611111111</v>
+        <v>-19.829861111111001</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -16698,7 +16926,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-20.9548611111111</v>
+        <v>-19.829861111111001</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16743,7 +16971,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-21.2881944444444</v>
+        <v>-20.163194444444301</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16788,7 +17016,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.4548611111111</v>
+        <v>-20.329861111111001</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16833,7 +17061,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.7881944444444</v>
+        <v>-20.663194444444301</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16878,7 +17106,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.7881944444444</v>
+        <v>-20.663194444444301</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16923,7 +17151,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.7881944444444</v>
+        <v>-20.663194444444301</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16968,7 +17196,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.7881944444444</v>
+        <v>-20.663194444444301</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17013,7 +17241,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.7881944444444</v>
+        <v>-20.663194444444301</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17058,7 +17286,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.1215277777777</v>
+        <v>-20.996527777777601</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17103,7 +17331,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.2881944444444</v>
+        <v>-21.163194444444301</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17148,7 +17376,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.6215277777777</v>
+        <v>-21.496527777777601</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17193,7 +17421,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.6215277777777</v>
+        <v>-21.496527777777601</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17238,7 +17466,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.6215277777777</v>
+        <v>-21.496527777777601</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17283,7 +17511,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.6215277777777</v>
+        <v>-21.496527777777601</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17328,7 +17556,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.6215277777777</v>
+        <v>-21.496527777777601</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17373,7 +17601,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.954861111111001</v>
+        <v>-21.829861111110901</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17418,7 +17646,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.1215277777777</v>
+        <v>-21.996527777777601</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17463,7 +17691,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.454861111111001</v>
+        <v>-22.329861111110901</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17508,7 +17736,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.454861111111001</v>
+        <v>-22.329861111110901</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17553,7 +17781,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.454861111111001</v>
+        <v>-22.329861111110901</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17598,7 +17826,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.454861111111001</v>
+        <v>-22.329861111110901</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17643,7 +17871,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.454861111111001</v>
+        <v>-22.329861111110901</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17688,7 +17916,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.788194444444301</v>
+        <v>-22.663194444444201</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17733,7 +17961,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.871527777777601</v>
+        <v>-22.746527777777501</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17778,7 +18006,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.871527777777601</v>
+        <v>-22.746527777777501</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17823,7 +18051,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.871527777777601</v>
+        <v>-22.746527777777501</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17868,7 +18096,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.871527777777601</v>
+        <v>-22.746527777777501</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17913,7 +18141,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.871527777777601</v>
+        <v>-22.746527777777501</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17958,7 +18186,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.871527777777601</v>
+        <v>-22.746527777777501</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18003,7 +18231,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-24.204861111110901</v>
+        <v>-23.079861111110802</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18048,7 +18276,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-24.288194444444201</v>
+        <v>-23.163194444444098</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -18079,7 +18307,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">November!F40</f>
-        <v>-20.9548611111111</v>
+        <v>-19.829861111111001</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -18200,7 +18428,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-24.2881944444444</v>
+        <v>-23.163194444444301</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -21627,9 +21855,9 @@
         <f>Mai!A23</f>
         <v>42509</v>
       </c>
-      <c r="O23" s="294" t="str">
+      <c r="O23" s="294">
         <f>IF(Mai!K23&gt;0,Mai!K23,"")</f>
-        <v/>
+        <v>0.35416666666666663</v>
       </c>
       <c r="P23" s="295" t="str">
         <f>IF(OR(Mai!C23="",Mai!J23&lt;&gt;""),UPPER(Mai!J23),"F")</f>
@@ -21931,9 +22159,9 @@
         <f>Mai!A25</f>
         <v>42511</v>
       </c>
-      <c r="O25" s="294" t="str">
+      <c r="O25" s="294">
         <f>IF(Mai!K25&gt;0,Mai!K25,"")</f>
-        <v/>
+        <v>0.35416666666666663</v>
       </c>
       <c r="P25" s="295" t="str">
         <f>IF(OR(Mai!C25="",Mai!J25&lt;&gt;""),UPPER(Mai!J25),"F")</f>
@@ -22387,9 +22615,9 @@
         <f>Mai!A28</f>
         <v>42514</v>
       </c>
-      <c r="O28" s="294" t="str">
+      <c r="O28" s="294">
         <f>IF(Mai!K28&gt;0,Mai!K28,"")</f>
-        <v/>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="P28" s="295" t="str">
         <f>IF(OR(Mai!C28="",Mai!J28&lt;&gt;""),UPPER(Mai!J28),"F")</f>
@@ -22539,9 +22767,9 @@
         <f>Mai!A29</f>
         <v>42515</v>
       </c>
-      <c r="O29" s="294" t="str">
+      <c r="O29" s="294">
         <f>IF(Mai!K29&gt;0,Mai!K29,"")</f>
-        <v/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="P29" s="295" t="str">
         <f>IF(OR(Mai!C29="",Mai!J29&lt;&gt;""),UPPER(Mai!J29),"F")</f>
@@ -23506,7 +23734,7 @@
       <c r="M36" s="317"/>
       <c r="N36" s="399">
         <f>Mai!F38</f>
-        <v>2.4826388888888888</v>
+        <v>3.6076388888888888</v>
       </c>
       <c r="O36" s="399"/>
       <c r="P36" s="318"/>
@@ -23554,7 +23782,7 @@
       <c r="AK36" s="317"/>
       <c r="AL36" s="319">
         <f t="shared" si="0"/>
-        <v>7.378472222222225</v>
+        <v>8.503472222222225</v>
       </c>
     </row>
     <row r="37" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -23587,7 +23815,7 @@
       <c r="M37" s="322"/>
       <c r="N37" s="394">
         <f ca="1">ROUND(N36-N35,10)</f>
-        <v>-0.68402777780000001</v>
+        <v>0.44097222219999999</v>
       </c>
       <c r="O37" s="394"/>
       <c r="P37" s="323"/>
@@ -23635,7 +23863,7 @@
       <c r="AK37" s="322"/>
       <c r="AL37" s="324">
         <f t="shared" ca="1" si="0"/>
-        <v>-24.288194444400002</v>
+        <v>-23.163194444400002</v>
       </c>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.25">
@@ -23668,7 +23896,7 @@
       <c r="M38" s="395"/>
       <c r="N38" s="395">
         <f>Mai!J40</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="O38" s="395"/>
       <c r="P38" s="395"/>
@@ -23716,7 +23944,7 @@
       <c r="AK38" s="395"/>
       <c r="AL38" s="326">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
@@ -28493,7 +28721,7 @@
       <c r="C2" s="346"/>
       <c r="D2" s="347">
         <f>Jahresübersicht!AL38</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="79" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
@@ -28514,7 +28742,7 @@
       <c r="C4" s="346"/>
       <c r="D4" s="349">
         <f>D2*D3</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="79" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
@@ -28541,7 +28769,7 @@
       <c r="C6" s="354"/>
       <c r="D6" s="355">
         <f>D5*D2</f>
-        <v>4.8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="79" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
@@ -34922,7 +35150,7 @@
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
@@ -37036,8 +37264,8 @@
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -38094,11 +38322,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D23" s="200"/>
-      <c r="E23" s="200"/>
+      <c r="D23" s="200">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E23" s="200">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F23" s="200"/>
       <c r="G23" s="200"/>
-      <c r="H23" s="201"/>
+      <c r="H23" s="201">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I23" s="202" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -38106,7 +38340,7 @@
       <c r="J23" s="203"/>
       <c r="K23" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.35416666666666663</v>
       </c>
       <c r="L23" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -38114,16 +38348,18 @@
       </c>
       <c r="M23" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.33333333333332998</v>
+        <v>2.0833333333330002E-2</v>
       </c>
       <c r="N23" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0.33333333333333298</v>
       </c>
-      <c r="O23" s="208"/>
+      <c r="O23" s="208" t="s">
+        <v>168</v>
+      </c>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.8784722222222201</v>
+        <v>2.23263888888888</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38168,7 +38404,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.8784722222222201</v>
+        <v>2.23263888888888</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38184,11 +38420,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D25" s="200"/>
-      <c r="E25" s="200"/>
+      <c r="D25" s="200">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E25" s="200">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F25" s="200"/>
       <c r="G25" s="200"/>
-      <c r="H25" s="201"/>
+      <c r="H25" s="201">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I25" s="202" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -38196,7 +38438,7 @@
       <c r="J25" s="203"/>
       <c r="K25" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.35416666666666663</v>
       </c>
       <c r="L25" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -38204,16 +38446,18 @@
       </c>
       <c r="M25" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.33333333333332998</v>
+        <v>2.0833333333330002E-2</v>
       </c>
       <c r="N25" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0.33333333333333298</v>
       </c>
-      <c r="O25" s="208"/>
+      <c r="O25" s="208" t="s">
+        <v>167</v>
+      </c>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.5451388888888899</v>
+        <v>2.2534722222222099</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38258,7 +38502,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.5451388888888899</v>
+        <v>2.2534722222222099</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38280,12 +38524,12 @@
       <c r="G27" s="200"/>
       <c r="H27" s="201"/>
       <c r="I27" s="202" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A27="","",IF(G27=0,IF(K27=0,"",IF(PauseGTime&lt;IF(E27&gt;D27,E27-D27,1-D27+E27),IF(H27&lt;PauseGWert,"!",""),IF(PauseKTime&lt;IF(E27&gt;D27,E27-D27,1-D27+E27),IF(H27&lt;PauseKWert,"!",""),""))),IF(PauseGTime&lt;IF(G27&gt;D27,G27-D27,1-D27+G27),IF(IF(F27&gt;E27,F27-E27,1-E27+F27)+H27+0.0000001&lt;PauseGWert,"!",""),IF(PauseKTime&lt;IF(G27&gt;D27,G27-D27,1-D27+G27),IF(IF(F27&gt;E27,F27-E27,1-E27+F27)+H27+0.0000001&lt;PauseKWert,"!",""),""))))</f>
         <v/>
       </c>
       <c r="J27" s="203"/>
       <c r="K27" s="204">
-        <f t="shared" si="3"/>
+        <f>IF(A27="","",IF(IF(D27&lt;E27,E27-D27,IF(E27="",0,E27-D27+1))+IF(F27&lt;G27,G27-F27,IF(G27="",0,G27-F27+1))-H27&gt;0,IF(D27&lt;E27,E27-D27,IF(E27="",0,E27-D27+1))+IF(F27&lt;G27,G27-F27,IF(G27="",0,G27-F27+1))-H27,0))</f>
         <v>0</v>
       </c>
       <c r="L27" s="205">
@@ -38303,7 +38547,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.5451388888888899</v>
+        <v>2.2534722222222099</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38319,19 +38563,23 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D28" s="200"/>
-      <c r="E28" s="200"/>
+      <c r="D28" s="200">
+        <v>0.75</v>
+      </c>
+      <c r="E28" s="200">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="F28" s="200"/>
       <c r="G28" s="200"/>
       <c r="H28" s="201"/>
       <c r="I28" s="202" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A28="","",IF(G28=0,IF(K28=0,"",IF(PauseGTime&lt;IF(E28&gt;D28,E28-D28,1-D28+E28),IF(H28&lt;PauseGWert,"!",""),IF(PauseKTime&lt;IF(E28&gt;D28,E28-D28,1-D28+E28),IF(H28&lt;PauseKWert,"!",""),""))),IF(PauseGTime&lt;IF(G28&gt;D28,G28-D28,1-D28+G28),IF(IF(F28&gt;E28,F28-E28,1-E28+F28)+H28+0.0000001&lt;PauseGWert,"!",""),IF(PauseKTime&lt;IF(G28&gt;D28,G28-D28,1-D28+G28),IF(IF(F28&gt;E28,F28-E28,1-E28+F28)+H28+0.0000001&lt;PauseKWert,"!",""),""))))</f>
         <v/>
       </c>
       <c r="J28" s="203"/>
       <c r="K28" s="204">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(A28="","",IF(IF(D28&lt;E28,E28-D28,IF(E28="",0,E28-D28+1))+IF(F28&lt;G28,G28-F28,IF(G28="",0,G28-F28+1))-H28&gt;0,IF(D28&lt;E28,E28-D28,IF(E28="",0,E28-D28+1))+IF(F28&lt;G28,G28-F28,IF(G28="",0,G28-F28+1))-H28,0))</f>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="L28" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -38339,16 +38587,18 @@
       </c>
       <c r="M28" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>8.3333333333329998E-2</v>
       </c>
       <c r="N28" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="O28" s="208"/>
+      <c r="O28" s="208" t="s">
+        <v>166</v>
+      </c>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.5451388888888899</v>
+        <v>2.3368055555555398</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38364,19 +38614,27 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D29" s="200"/>
-      <c r="E29" s="200"/>
-      <c r="F29" s="200"/>
-      <c r="G29" s="200"/>
+      <c r="D29" s="200">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E29" s="200">
+        <v>0.625</v>
+      </c>
+      <c r="F29" s="200">
+        <v>0.75</v>
+      </c>
+      <c r="G29" s="200">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="H29" s="201"/>
       <c r="I29" s="202" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A29="","",IF(G29=0,IF(K29=0,"",IF(PauseGTime&lt;IF(E29&gt;D29,E29-D29,1-D29+E29),IF(H29&lt;PauseGWert,"!",""),IF(PauseKTime&lt;IF(E29&gt;D29,E29-D29,1-D29+E29),IF(H29&lt;PauseKWert,"!",""),""))),IF(PauseGTime&lt;IF(G29&gt;D29,G29-D29,1-D29+G29),IF(IF(F29&gt;E29,F29-E29,1-E29+F29)+H29+0.0000001&lt;PauseGWert,"!",""),IF(PauseKTime&lt;IF(G29&gt;D29,G29-D29,1-D29+G29),IF(IF(F29&gt;E29,F29-E29,1-E29+F29)+H29+0.0000001&lt;PauseKWert,"!",""),""))))</f>
         <v/>
       </c>
       <c r="J29" s="203"/>
       <c r="K29" s="204">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(A29="","",IF(IF(D29&lt;E29,E29-D29,IF(E29="",0,E29-D29+1))+IF(F29&lt;G29,G29-F29,IF(G29="",0,G29-F29+1))-H29&gt;0,IF(D29&lt;E29,E29-D29,IF(E29="",0,E29-D29+1))+IF(F29&lt;G29,G29-F29,IF(G29="",0,G29-F29+1))-H29,0))</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="L29" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -38384,16 +38642,18 @@
       </c>
       <c r="M29" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>0.33333333333332998</v>
       </c>
       <c r="N29" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="O29" s="208"/>
+      <c r="O29" s="208" t="s">
+        <v>169</v>
+      </c>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.5451388888888899</v>
+        <v>2.6701388888888702</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38438,7 +38698,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.21180555555556</v>
+        <v>2.3368055555555398</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38483,7 +38743,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0451388888888899</v>
+        <v>2.1701388888888702</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38528,7 +38788,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.71180555555556002</v>
+        <v>1.83680555555554</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38573,7 +38833,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.71180555555556002</v>
+        <v>1.83680555555554</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38618,7 +38878,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>0.71180555555556002</v>
+        <v>1.83680555555554</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -38714,7 +38974,7 @@
       </c>
       <c r="F38" s="246">
         <f>SUM(K4:K34)</f>
-        <v>2.4826388888888888</v>
+        <v>3.6076388888888888</v>
       </c>
       <c r="G38" s="163"/>
       <c r="H38" s="163"/>
@@ -38770,14 +39030,14 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>0.71180555555556002</v>
+        <v>1.83680555555556</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
       <c r="I40" s="258"/>
       <c r="J40" s="259">
         <f>COUNTIF(K4:K34,"&gt;0")-IF(Voreinstellungen!C28="XTRA",COUNTIF(J4:J34,Voreinstellungen!B28),0)-IF(Voreinstellungen!C29="XTRA",COUNTIF(J4:J34,Voreinstellungen!B29),0)-IF(Voreinstellungen!C30="XTRA",COUNTIF(J4:J34,Voreinstellungen!B30),0)-IF(Voreinstellungen!C31="XTRA",COUNTIF(J4:J34,Voreinstellungen!B31),0)-IF(Voreinstellungen!C32="XTRA",COUNTIF(J4:J34,Voreinstellungen!B32),0)-IF(Voreinstellungen!C33="XTRA",COUNTIF(J4:J34,Voreinstellungen!B33),0)-COUNTIF(J4:J34,"H")</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K40" s="382" t="s">
         <v>112</v>
@@ -39000,7 +39260,7 @@
       <formula>MOD(J36,1)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:M34 O4:P13 O16:P34 P14:P15">
+  <conditionalFormatting sqref="A4:M34 O4:P13 P14:P15 O16:P34">
     <cfRule type="expression" dxfId="104" priority="3">
       <formula>WEEKDAY($A4,2)=6</formula>
     </cfRule>
@@ -39227,7 +39487,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>0.71180555555556002</v>
+        <v>1.83680555555556</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39272,7 +39532,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>0.71180555555556002</v>
+        <v>1.83680555555556</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39317,7 +39577,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.37847222222222998</v>
+        <v>1.5034722222222301</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39362,7 +39622,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.21180555555555999</v>
+        <v>1.33680555555556</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39407,7 +39667,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.12152777777777</v>
+        <v>1.0034722222222301</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39452,7 +39712,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.12152777777777</v>
+        <v>1.0034722222222301</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39497,7 +39757,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.12152777777777</v>
+        <v>1.0034722222222301</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39542,7 +39802,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.12152777777777</v>
+        <v>1.0034722222222301</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39587,7 +39847,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.12152777777777</v>
+        <v>1.0034722222222301</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39632,7 +39892,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.4548611111111</v>
+        <v>0.67013888888890005</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39677,7 +39937,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.62152777777777002</v>
+        <v>0.50347222222222998</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39722,7 +39982,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.95486111111109995</v>
+        <v>0.1701388888889</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39767,7 +40027,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.95486111111109995</v>
+        <v>0.1701388888889</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39812,7 +40072,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.95486111111109995</v>
+        <v>0.1701388888889</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39857,7 +40117,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.95486111111109995</v>
+        <v>0.1701388888889</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39902,7 +40162,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.95486111111109995</v>
+        <v>0.1701388888889</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39947,7 +40207,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.28819444444443</v>
+        <v>-0.16319444444442999</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39992,7 +40252,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4548611111111001</v>
+        <v>-0.3298611111111</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40037,7 +40297,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.78819444444443</v>
+        <v>-0.66319444444442999</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40082,7 +40342,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.78819444444443</v>
+        <v>-0.66319444444442999</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40127,7 +40387,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.78819444444443</v>
+        <v>-0.66319444444442999</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40172,7 +40432,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.78819444444443</v>
+        <v>-0.66319444444442999</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40217,7 +40477,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.78819444444443</v>
+        <v>-0.66319444444442999</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40262,7 +40522,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.1215277777777599</v>
+        <v>-0.99652777777776003</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40307,7 +40567,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.28819444444443</v>
+        <v>-1.16319444444443</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40352,7 +40612,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.6215277777777599</v>
+        <v>-1.4965277777777599</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40397,7 +40657,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.6215277777777599</v>
+        <v>-1.4965277777777599</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40442,7 +40702,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.6215277777777599</v>
+        <v>-1.4965277777777599</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40487,7 +40747,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.6215277777777599</v>
+        <v>-1.4965277777777599</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40532,7 +40792,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.6215277777777599</v>
+        <v>-1.4965277777777599</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40608,7 +40868,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">Mai!F40</f>
-        <v>0.71180555555556002</v>
+        <v>1.83680555555556</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -40729,7 +40989,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-2.6215277777777701</v>
+        <v>-1.4965277777777699</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -41178,7 +41438,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-2.9548611111111001</v>
+        <v>-1.8298611111111001</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41223,7 +41483,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-3.1215277777777701</v>
+        <v>-1.9965277777777699</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41268,7 +41528,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.4548611111111001</v>
+        <v>-2.3298611111111001</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41313,7 +41573,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.4548611111111001</v>
+        <v>-2.3298611111111001</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41358,7 +41618,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.4548611111111001</v>
+        <v>-2.3298611111111001</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41403,7 +41663,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.4548611111111001</v>
+        <v>-2.3298611111111001</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41448,7 +41708,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.4548611111111001</v>
+        <v>-2.3298611111111001</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41493,7 +41753,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.78819444444443</v>
+        <v>-2.66319444444443</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41538,7 +41798,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.9548611111111001</v>
+        <v>-2.8298611111111001</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41583,7 +41843,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.2881944444444304</v>
+        <v>-3.16319444444443</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41628,7 +41888,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.2881944444444304</v>
+        <v>-3.16319444444443</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41673,7 +41933,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.2881944444444304</v>
+        <v>-3.16319444444443</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41718,7 +41978,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.2881944444444304</v>
+        <v>-3.16319444444443</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41763,7 +42023,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.2881944444444304</v>
+        <v>-3.16319444444443</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41808,7 +42068,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.6215277777777599</v>
+        <v>-3.4965277777777599</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41853,7 +42113,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.7881944444444304</v>
+        <v>-3.66319444444443</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41898,7 +42158,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.1215277777777599</v>
+        <v>-3.9965277777777599</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41943,7 +42203,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.1215277777777599</v>
+        <v>-3.9965277777777599</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41988,7 +42248,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.1215277777777599</v>
+        <v>-3.9965277777777599</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42033,7 +42293,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.1215277777777599</v>
+        <v>-3.9965277777777599</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42078,7 +42338,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.1215277777777599</v>
+        <v>-3.9965277777777599</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42123,7 +42383,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.4548611111110903</v>
+        <v>-4.3298611111110903</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42168,7 +42428,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.6215277777777599</v>
+        <v>-4.4965277777777599</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42213,7 +42473,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.9548611111110903</v>
+        <v>-4.8298611111110903</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42258,7 +42518,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.9548611111110903</v>
+        <v>-4.8298611111110903</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42303,7 +42563,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.9548611111110903</v>
+        <v>-4.8298611111110903</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42348,7 +42608,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.9548611111110903</v>
+        <v>-4.8298611111110903</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42393,7 +42653,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.9548611111110903</v>
+        <v>-4.8298611111110903</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42438,7 +42698,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.2881944444444198</v>
+        <v>-5.1631944444444198</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42483,7 +42743,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.4548611111110903</v>
+        <v>-5.3298611111110903</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42528,7 +42788,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.7881944444444198</v>
+        <v>-5.6631944444444198</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -42559,7 +42819,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">Juni!F40</f>
-        <v>-2.6215277777777701</v>
+        <v>-1.4965277777777699</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -42680,7 +42940,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-6.7881944444444402</v>
+        <v>-5.6631944444444304</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>

</xml_diff>

<commit_message>
This contains the last comments about the RTOS SM Implementation
</commit_message>
<xml_diff>
--- a/Admin/Arbeitszeiterfassung-2020-jcr.xlsx
+++ b/Admin/Arbeitszeiterfassung-2020-jcr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Projektarbeit_Docs\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633ACE76-105D-4CF7-9985-795B2ACFA4D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3922E64-4734-42A9-90A3-8C2A3334847F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Voreinstellungen" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="177">
   <si>
     <t>Benutzer-Voreinstellungen</t>
   </si>
@@ -659,6 +659,27 @@
   </si>
   <si>
     <t>PCB Aligned-Final Routing=Results!</t>
+  </si>
+  <si>
+    <t>Results=PCB design sent to manufacture</t>
+  </si>
+  <si>
+    <t>No Results=SPI communication started and mofifiaction of pcb</t>
+  </si>
+  <si>
+    <t>Results=SPI communication with DMA</t>
+  </si>
+  <si>
+    <t>No Results: SMs started</t>
+  </si>
+  <si>
+    <t>Results: New PCB design started and SMs</t>
+  </si>
+  <si>
+    <t>Results: SM with functions defined</t>
+  </si>
+  <si>
+    <t>Results:osEvents os Timers ECAT Test SM working</t>
   </si>
 </sst>
 </file>
@@ -7149,6 +7170,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3BC5FC8-5059-490F-869F-CF1AE30E10C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{997D372B-4AFE-47BC-9878-90E1FF02BEDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8157,6 +8286,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8A49221-4714-4B40-B30E-3B08A9DFBC35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96610FCB-FE52-4F47-AAA0-6E4B885216A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9122,7 +9359,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-5.6631944444444304</v>
+        <v>-3.48263888888888</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9167,7 +9404,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-5.6631944444444304</v>
+        <v>-3.48263888888888</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9212,7 +9449,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.6631944444444304</v>
+        <v>-3.48263888888888</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9257,7 +9494,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.6631944444444304</v>
+        <v>-3.48263888888888</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9302,7 +9539,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.9965277777777599</v>
+        <v>-3.8159722222222099</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9347,7 +9584,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.1631944444444304</v>
+        <v>-3.98263888888888</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9392,7 +9629,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.4965277777777599</v>
+        <v>-4.3159722222222099</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9437,7 +9674,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.4965277777777599</v>
+        <v>-4.3159722222222099</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9482,7 +9719,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.4965277777777599</v>
+        <v>-4.3159722222222099</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9527,7 +9764,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.4965277777777599</v>
+        <v>-4.3159722222222099</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9572,7 +9809,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.4965277777777599</v>
+        <v>-4.3159722222222099</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9617,7 +9854,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.8298611111110903</v>
+        <v>-4.6493055555555403</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9662,7 +9899,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.9965277777777599</v>
+        <v>-4.8159722222222099</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9707,7 +9944,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.3298611111110903</v>
+        <v>-5.1493055555555403</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9752,7 +9989,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.3298611111110903</v>
+        <v>-5.1493055555555403</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9797,7 +10034,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.3298611111110903</v>
+        <v>-5.1493055555555403</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9842,7 +10079,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.3298611111110903</v>
+        <v>-5.1493055555555403</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9887,7 +10124,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.3298611111110903</v>
+        <v>-5.1493055555555403</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9932,7 +10169,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.6631944444444198</v>
+        <v>-5.4826388888888697</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9977,7 +10214,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.8298611111110903</v>
+        <v>-5.6493055555555403</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10022,7 +10259,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.1631944444444198</v>
+        <v>-5.9826388888888697</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10067,7 +10304,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.1631944444444198</v>
+        <v>-5.9826388888888697</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10112,7 +10349,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.1631944444444198</v>
+        <v>-5.9826388888888697</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10157,7 +10394,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.1631944444444198</v>
+        <v>-5.9826388888888697</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10202,7 +10439,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.1631944444444198</v>
+        <v>-5.9826388888888697</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10247,7 +10484,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.4965277777777501</v>
+        <v>-6.3159722222222001</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10292,7 +10529,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.6631944444444198</v>
+        <v>-6.4826388888888697</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10337,7 +10574,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.9965277777777501</v>
+        <v>-6.8159722222222001</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10382,7 +10619,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.9965277777777501</v>
+        <v>-6.8159722222222001</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10427,7 +10664,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.9965277777777501</v>
+        <v>-6.8159722222222001</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10472,7 +10709,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.9965277777777501</v>
+        <v>-6.8159722222222001</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -10503,7 +10740,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">Juli!F40</f>
-        <v>-5.6631944444444304</v>
+        <v>-3.48263888888888</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -10624,7 +10861,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-8.9965277777777608</v>
+        <v>-6.8159722222222099</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -11073,7 +11310,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-8.9965277777777608</v>
+        <v>-6.8159722222222099</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11118,7 +11355,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-9.3298611111110894</v>
+        <v>-7.1493055555555403</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11163,7 +11400,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.4965277777777608</v>
+        <v>-7.3159722222222099</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11208,7 +11445,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.8298611111110894</v>
+        <v>-7.6493055555555403</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11253,7 +11490,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.8298611111110894</v>
+        <v>-7.6493055555555403</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11298,7 +11535,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.8298611111110894</v>
+        <v>-7.6493055555555403</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11343,7 +11580,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.8298611111110894</v>
+        <v>-7.6493055555555403</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11388,7 +11625,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.8298611111110894</v>
+        <v>-7.6493055555555403</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11433,7 +11670,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.1631944444444</v>
+        <v>-7.9826388888888697</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11478,7 +11715,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.3298611111111</v>
+        <v>-8.1493055555555394</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11523,7 +11760,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.6631944444444</v>
+        <v>-8.4826388888888697</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11568,7 +11805,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.6631944444444</v>
+        <v>-8.4826388888888697</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11613,7 +11850,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.6631944444444</v>
+        <v>-8.4826388888888697</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11658,7 +11895,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.6631944444444</v>
+        <v>-8.4826388888888697</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11703,7 +11940,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.6631944444444</v>
+        <v>-8.4826388888888697</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11748,7 +11985,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.9965277777777</v>
+        <v>-8.8159722222222001</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11793,7 +12030,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.1631944444444</v>
+        <v>-8.9826388888888697</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11838,7 +12075,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.4965277777777</v>
+        <v>-9.3159722222222001</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11883,7 +12120,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.4965277777777</v>
+        <v>-9.3159722222222001</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11928,7 +12165,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.4965277777777</v>
+        <v>-9.3159722222222001</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11973,7 +12210,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.4965277777777</v>
+        <v>-9.3159722222222001</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12018,7 +12255,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.4965277777777</v>
+        <v>-9.3159722222222001</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12063,7 +12300,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.829861111111001</v>
+        <v>-9.6493055555555305</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12108,7 +12345,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.9965277777777</v>
+        <v>-9.8159722222222001</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12153,7 +12390,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.329861111111001</v>
+        <v>-10.1493055555555</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12198,7 +12435,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.329861111111001</v>
+        <v>-10.1493055555555</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12243,7 +12480,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.329861111111001</v>
+        <v>-10.1493055555555</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12288,7 +12525,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.329861111111001</v>
+        <v>-10.1493055555555</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12333,7 +12570,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.329861111111001</v>
+        <v>-10.1493055555555</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12378,7 +12615,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.663194444444301</v>
+        <v>-10.4826388888888</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12454,7 +12691,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">August!F40</f>
-        <v>-8.9965277777777608</v>
+        <v>-6.8159722222222099</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -12575,7 +12812,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-12.6631944444444</v>
+        <v>-10.4826388888889</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -13024,7 +13261,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-12.8298611111111</v>
+        <v>-10.6493055555556</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13069,7 +13306,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-13.1631944444444</v>
+        <v>-10.9826388888889</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13114,7 +13351,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.1631944444444</v>
+        <v>-10.9826388888889</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13159,7 +13396,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.1631944444444</v>
+        <v>-10.9826388888889</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13204,7 +13441,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.1631944444444</v>
+        <v>-10.9826388888889</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13249,7 +13486,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.1631944444444</v>
+        <v>-10.9826388888889</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13294,7 +13531,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.4965277777777</v>
+        <v>-11.3159722222222</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13339,7 +13576,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.6631944444444</v>
+        <v>-11.4826388888889</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13384,7 +13621,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.9965277777777</v>
+        <v>-11.8159722222222</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13429,7 +13666,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.9965277777777</v>
+        <v>-11.8159722222222</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13474,7 +13711,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.9965277777777</v>
+        <v>-11.8159722222222</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13519,7 +13756,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.9965277777777</v>
+        <v>-11.8159722222222</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13564,7 +13801,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.9965277777777</v>
+        <v>-11.8159722222222</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13609,7 +13846,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.329861111111001</v>
+        <v>-12.1493055555555</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13654,7 +13891,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.4965277777777</v>
+        <v>-12.3159722222222</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13699,7 +13936,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.829861111111001</v>
+        <v>-12.6493055555555</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13744,7 +13981,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.829861111111001</v>
+        <v>-12.6493055555555</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13789,7 +14026,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.829861111111001</v>
+        <v>-12.6493055555555</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13834,7 +14071,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.829861111111001</v>
+        <v>-12.6493055555555</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13879,7 +14116,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.829861111111001</v>
+        <v>-12.6493055555555</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13924,7 +14161,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.163194444444301</v>
+        <v>-12.9826388888888</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13969,7 +14206,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.329861111111001</v>
+        <v>-13.1493055555555</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14014,7 +14251,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.663194444444301</v>
+        <v>-13.4826388888888</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14059,7 +14296,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.663194444444301</v>
+        <v>-13.4826388888888</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14104,7 +14341,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.663194444444301</v>
+        <v>-13.4826388888888</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14149,7 +14386,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.663194444444301</v>
+        <v>-13.4826388888888</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14194,7 +14431,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.663194444444301</v>
+        <v>-13.4826388888888</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14239,7 +14476,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.996527777777599</v>
+        <v>-13.815972222222101</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14284,7 +14521,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.163194444444301</v>
+        <v>-13.9826388888888</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14329,7 +14566,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.496527777777601</v>
+        <v>-14.315972222222101</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14374,7 +14611,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.496527777777601</v>
+        <v>-14.315972222222101</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -14405,7 +14642,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">September!F40</f>
-        <v>-12.6631944444444</v>
+        <v>-10.4826388888889</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -14526,7 +14763,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-16.4965277777777</v>
+        <v>-14.3159722222222</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -14975,7 +15212,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-16.4965277777777</v>
+        <v>-14.3159722222222</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15020,7 +15257,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-16.4965277777777</v>
+        <v>-14.3159722222222</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15065,7 +15302,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.4965277777777</v>
+        <v>-14.3159722222222</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15110,7 +15347,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.829861111111001</v>
+        <v>-14.6493055555555</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15155,7 +15392,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.9965277777777</v>
+        <v>-14.8159722222222</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15200,7 +15437,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.329861111111001</v>
+        <v>-15.1493055555555</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15245,7 +15482,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.329861111111001</v>
+        <v>-15.1493055555555</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15290,7 +15527,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.329861111111001</v>
+        <v>-15.1493055555555</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15335,7 +15572,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.329861111111001</v>
+        <v>-15.1493055555555</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15380,7 +15617,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.329861111111001</v>
+        <v>-15.1493055555555</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15425,7 +15662,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.663194444444301</v>
+        <v>-15.4826388888888</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15470,7 +15707,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.829861111111001</v>
+        <v>-15.6493055555555</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15515,7 +15752,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.163194444444301</v>
+        <v>-15.9826388888888</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15560,7 +15797,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.163194444444301</v>
+        <v>-15.9826388888888</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15605,7 +15842,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.163194444444301</v>
+        <v>-15.9826388888888</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15650,7 +15887,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.163194444444301</v>
+        <v>-15.9826388888888</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15695,7 +15932,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.163194444444301</v>
+        <v>-15.9826388888888</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15740,7 +15977,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.496527777777601</v>
+        <v>-16.315972222222101</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15785,7 +16022,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.663194444444301</v>
+        <v>-16.4826388888888</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15830,7 +16067,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.996527777777601</v>
+        <v>-16.815972222222101</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15875,7 +16112,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.996527777777601</v>
+        <v>-16.815972222222101</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15920,7 +16157,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.996527777777601</v>
+        <v>-16.815972222222101</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15965,7 +16202,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.996527777777601</v>
+        <v>-16.815972222222101</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16010,7 +16247,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.996527777777601</v>
+        <v>-16.815972222222101</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16055,7 +16292,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.329861111110901</v>
+        <v>-17.149305555555401</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16100,7 +16337,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.496527777777601</v>
+        <v>-17.315972222222101</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16145,7 +16382,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.829861111110901</v>
+        <v>-17.649305555555401</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16190,7 +16427,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.829861111110901</v>
+        <v>-17.649305555555401</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16235,7 +16472,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.829861111110901</v>
+        <v>-17.649305555555401</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16280,7 +16517,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.829861111110901</v>
+        <v>-17.649305555555401</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16356,7 +16593,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">Oktober!F40</f>
-        <v>-16.4965277777777</v>
+        <v>-14.3159722222222</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -16477,7 +16714,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-19.829861111111001</v>
+        <v>-17.6493055555555</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -16926,7 +17163,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-19.829861111111001</v>
+        <v>-17.6493055555555</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16971,7 +17208,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-20.163194444444301</v>
+        <v>-17.9826388888888</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17016,7 +17253,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.329861111111001</v>
+        <v>-18.1493055555555</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17061,7 +17298,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.663194444444301</v>
+        <v>-18.4826388888888</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17106,7 +17343,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.663194444444301</v>
+        <v>-18.4826388888888</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17151,7 +17388,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.663194444444301</v>
+        <v>-18.4826388888888</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17196,7 +17433,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.663194444444301</v>
+        <v>-18.4826388888888</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17241,7 +17478,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.663194444444301</v>
+        <v>-18.4826388888888</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17286,7 +17523,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-20.996527777777601</v>
+        <v>-18.815972222222101</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17331,7 +17568,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.163194444444301</v>
+        <v>-18.9826388888888</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17376,7 +17613,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.496527777777601</v>
+        <v>-19.315972222222101</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17421,7 +17658,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.496527777777601</v>
+        <v>-19.315972222222101</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17466,7 +17703,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.496527777777601</v>
+        <v>-19.315972222222101</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17511,7 +17748,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.496527777777601</v>
+        <v>-19.315972222222101</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17556,7 +17793,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.496527777777601</v>
+        <v>-19.315972222222101</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17601,7 +17838,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.829861111110901</v>
+        <v>-19.649305555555401</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17646,7 +17883,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-21.996527777777601</v>
+        <v>-19.815972222222101</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17691,7 +17928,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.329861111110901</v>
+        <v>-20.149305555555401</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17736,7 +17973,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.329861111110901</v>
+        <v>-20.149305555555401</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17781,7 +18018,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.329861111110901</v>
+        <v>-20.149305555555401</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17826,7 +18063,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.329861111110901</v>
+        <v>-20.149305555555401</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17871,7 +18108,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.329861111110901</v>
+        <v>-20.149305555555401</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17916,7 +18153,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.663194444444201</v>
+        <v>-20.482638888888701</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17961,7 +18198,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.746527777777501</v>
+        <v>-20.565972222222001</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18006,7 +18243,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.746527777777501</v>
+        <v>-20.565972222222001</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18051,7 +18288,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.746527777777501</v>
+        <v>-20.565972222222001</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18096,7 +18333,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.746527777777501</v>
+        <v>-20.565972222222001</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18141,7 +18378,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.746527777777501</v>
+        <v>-20.565972222222001</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18186,7 +18423,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-22.746527777777501</v>
+        <v>-20.565972222222001</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18231,7 +18468,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.079861111110802</v>
+        <v>-20.899305555555301</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18276,7 +18513,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-23.163194444444098</v>
+        <v>-20.982638888888602</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -18307,7 +18544,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">November!F40</f>
-        <v>-19.829861111111001</v>
+        <v>-17.6493055555555</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -18428,7 +18665,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-23.163194444444301</v>
+        <v>-20.9826388888888</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -18979,9 +19216,9 @@
         <f>Juni!A4</f>
         <v>42521</v>
       </c>
-      <c r="R4" s="285" t="str">
+      <c r="R4" s="285">
         <f>IF(Juni!K4&gt;0,Juni!K4,"")</f>
-        <v/>
+        <v>0.29166666666666657</v>
       </c>
       <c r="S4" s="290" t="str">
         <f>IF(OR(Juni!C4="",Juni!J4&lt;&gt;""),UPPER(Juni!J4),"F")</f>
@@ -19283,9 +19520,9 @@
         <f>Juni!A6</f>
         <v>42523</v>
       </c>
-      <c r="R6" s="294" t="str">
+      <c r="R6" s="294">
         <f>IF(Juni!K6&gt;0,Juni!K6,"")</f>
-        <v/>
+        <v>0.35416666666666663</v>
       </c>
       <c r="S6" s="299" t="str">
         <f>IF(OR(Juni!C6="",Juni!J6&lt;&gt;""),UPPER(Juni!J6),"F")</f>
@@ -19435,9 +19672,9 @@
         <f>Juni!A7</f>
         <v>42524</v>
       </c>
-      <c r="R7" s="294" t="str">
+      <c r="R7" s="294">
         <f>IF(Juni!K7&gt;0,Juni!K7,"")</f>
-        <v/>
+        <v>0.25694444444444436</v>
       </c>
       <c r="S7" s="299" t="str">
         <f>IF(OR(Juni!C7="",Juni!J7&lt;&gt;""),UPPER(Juni!J7),"F")</f>
@@ -19587,9 +19824,9 @@
         <f>Juni!A8</f>
         <v>42525</v>
       </c>
-      <c r="R8" s="294" t="str">
+      <c r="R8" s="294">
         <f>IF(Juni!K8&gt;0,Juni!K8,"")</f>
-        <v/>
+        <v>0.36111111111111105</v>
       </c>
       <c r="S8" s="299" t="str">
         <f>IF(OR(Juni!C8="",Juni!J8&lt;&gt;""),UPPER(Juni!J8),"F")</f>
@@ -22919,9 +23156,9 @@
         <f>Mai!A30</f>
         <v>42516</v>
       </c>
-      <c r="O30" s="294" t="str">
+      <c r="O30" s="294">
         <f>IF(Mai!K30&gt;0,Mai!K30,"")</f>
-        <v/>
+        <v>0.35416666666666674</v>
       </c>
       <c r="P30" s="295" t="str">
         <f>IF(OR(Mai!C30="",Mai!J30&lt;&gt;""),UPPER(Mai!J30),"F")</f>
@@ -23071,9 +23308,9 @@
         <f>Mai!A31</f>
         <v>42517</v>
       </c>
-      <c r="O31" s="294" t="str">
+      <c r="O31" s="294">
         <f>IF(Mai!K31&gt;0,Mai!K31,"")</f>
-        <v/>
+        <v>0.22916666666666666</v>
       </c>
       <c r="P31" s="295" t="str">
         <f>IF(OR(Mai!C31="",Mai!J31&lt;&gt;""),UPPER(Mai!J31),"F")</f>
@@ -23223,9 +23460,9 @@
         <f>Mai!A32</f>
         <v>42518</v>
       </c>
-      <c r="O32" s="294" t="str">
+      <c r="O32" s="294">
         <f>IF(Mai!K32&gt;0,Mai!K32,"")</f>
-        <v/>
+        <v>0.33333333333333337</v>
       </c>
       <c r="P32" s="295" t="str">
         <f>IF(OR(Mai!C32="",Mai!J32&lt;&gt;""),UPPER(Mai!J32),"F")</f>
@@ -23734,13 +23971,13 @@
       <c r="M36" s="317"/>
       <c r="N36" s="399">
         <f>Mai!F38</f>
-        <v>3.6076388888888888</v>
+        <v>4.5243055555555554</v>
       </c>
       <c r="O36" s="399"/>
       <c r="P36" s="318"/>
       <c r="Q36" s="398">
         <f>Juni!F38</f>
-        <v>0</v>
+        <v>1.2638888888888888</v>
       </c>
       <c r="R36" s="398"/>
       <c r="S36" s="317"/>
@@ -23782,7 +24019,7 @@
       <c r="AK36" s="317"/>
       <c r="AL36" s="319">
         <f t="shared" si="0"/>
-        <v>8.503472222222225</v>
+        <v>10.684027777777782</v>
       </c>
     </row>
     <row r="37" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -23815,13 +24052,13 @@
       <c r="M37" s="322"/>
       <c r="N37" s="394">
         <f ca="1">ROUND(N36-N35,10)</f>
-        <v>0.44097222219999999</v>
+        <v>1.3576388889</v>
       </c>
       <c r="O37" s="394"/>
       <c r="P37" s="323"/>
       <c r="Q37" s="393">
         <f ca="1">ROUND(Q36-Q35,10)</f>
-        <v>-3.3333333333000001</v>
+        <v>-2.0694444444000002</v>
       </c>
       <c r="R37" s="393"/>
       <c r="S37" s="322"/>
@@ -23863,7 +24100,7 @@
       <c r="AK37" s="322"/>
       <c r="AL37" s="324">
         <f t="shared" ca="1" si="0"/>
-        <v>-23.163194444400002</v>
+        <v>-20.9826388888</v>
       </c>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.25">
@@ -23896,13 +24133,13 @@
       <c r="M38" s="395"/>
       <c r="N38" s="395">
         <f>Mai!J40</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="O38" s="395"/>
       <c r="P38" s="395"/>
       <c r="Q38" s="395">
         <f>Juni!J40</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R38" s="395"/>
       <c r="S38" s="395"/>
@@ -23944,7 +24181,7 @@
       <c r="AK38" s="395"/>
       <c r="AL38" s="326">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
@@ -28721,7 +28958,7 @@
       <c r="C2" s="346"/>
       <c r="D2" s="347">
         <f>Jahresübersicht!AL38</f>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="79" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
@@ -28742,7 +28979,7 @@
       <c r="C4" s="346"/>
       <c r="D4" s="349">
         <f>D2*D3</f>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="79" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
@@ -28769,7 +29006,7 @@
       <c r="C6" s="354"/>
       <c r="D6" s="355">
         <f>D5*D2</f>
-        <v>6</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="79" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
@@ -37263,9 +37500,9 @@
   </sheetPr>
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O31" sqref="O31"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -38669,11 +38906,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D30" s="200"/>
-      <c r="E30" s="200"/>
+      <c r="D30" s="200">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E30" s="200">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="F30" s="200"/>
       <c r="G30" s="200"/>
-      <c r="H30" s="201"/>
+      <c r="H30" s="201">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I30" s="202" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -38681,7 +38924,7 @@
       <c r="J30" s="203"/>
       <c r="K30" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.35416666666666674</v>
       </c>
       <c r="L30" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -38689,16 +38932,18 @@
       </c>
       <c r="M30" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.33333333333332998</v>
+        <v>2.0833333333330002E-2</v>
       </c>
       <c r="N30" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0.33333333333333298</v>
       </c>
-      <c r="O30" s="208"/>
+      <c r="O30" s="208" t="s">
+        <v>170</v>
+      </c>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>2.3368055555555398</v>
+        <v>2.6909722222222001</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38714,11 +38959,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D31" s="200"/>
-      <c r="E31" s="200"/>
+      <c r="D31" s="200">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E31" s="200">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F31" s="200"/>
       <c r="G31" s="200"/>
-      <c r="H31" s="201"/>
+      <c r="H31" s="201">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I31" s="202" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -38726,7 +38977,7 @@
       <c r="J31" s="203"/>
       <c r="K31" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="L31" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -38734,16 +38985,18 @@
       </c>
       <c r="M31" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.16666666666666999</v>
+        <v>6.25E-2</v>
       </c>
       <c r="N31" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0.16666666666666699</v>
       </c>
-      <c r="O31" s="208"/>
+      <c r="O31" s="208" t="s">
+        <v>171</v>
+      </c>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>2.1701388888888702</v>
+        <v>2.7534722222222001</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38759,11 +39012,17 @@
         <f>IF(ISERROR(VLOOKUP(A32,Feiertage,2,0)),"",(VLOOKUP(A32,Feiertage,2,0)))</f>
         <v/>
       </c>
-      <c r="D32" s="200"/>
-      <c r="E32" s="200"/>
+      <c r="D32" s="200">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E32" s="200">
+        <v>0.75</v>
+      </c>
       <c r="F32" s="200"/>
       <c r="G32" s="200"/>
-      <c r="H32" s="201"/>
+      <c r="H32" s="201">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I32" s="202" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -38771,7 +39030,7 @@
       <c r="J32" s="203"/>
       <c r="K32" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="L32" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -38779,16 +39038,18 @@
       </c>
       <c r="M32" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.33333333333332998</v>
+        <v>0</v>
       </c>
       <c r="N32" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0.33333333333333298</v>
       </c>
-      <c r="O32" s="208"/>
+      <c r="O32" s="208" t="s">
+        <v>172</v>
+      </c>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.83680555555554</v>
+        <v>2.7534722222222001</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38833,7 +39094,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.83680555555554</v>
+        <v>2.7534722222222001</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38878,7 +39139,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>1.83680555555554</v>
+        <v>2.7534722222222001</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -38974,7 +39235,7 @@
       </c>
       <c r="F38" s="246">
         <f>SUM(K4:K34)</f>
-        <v>3.6076388888888888</v>
+        <v>4.5243055555555554</v>
       </c>
       <c r="G38" s="163"/>
       <c r="H38" s="163"/>
@@ -39030,14 +39291,14 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>1.83680555555556</v>
+        <v>2.7534722222222299</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
       <c r="I40" s="258"/>
       <c r="J40" s="259">
         <f>COUNTIF(K4:K34,"&gt;0")-IF(Voreinstellungen!C28="XTRA",COUNTIF(J4:J34,Voreinstellungen!B28),0)-IF(Voreinstellungen!C29="XTRA",COUNTIF(J4:J34,Voreinstellungen!B29),0)-IF(Voreinstellungen!C30="XTRA",COUNTIF(J4:J34,Voreinstellungen!B30),0)-IF(Voreinstellungen!C31="XTRA",COUNTIF(J4:J34,Voreinstellungen!B31),0)-IF(Voreinstellungen!C32="XTRA",COUNTIF(J4:J34,Voreinstellungen!B32),0)-IF(Voreinstellungen!C33="XTRA",COUNTIF(J4:J34,Voreinstellungen!B33),0)-COUNTIF(J4:J34,"H")</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K40" s="382" t="s">
         <v>112</v>
@@ -39260,7 +39521,7 @@
       <formula>MOD(J36,1)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:M34 O4:P13 P14:P15 O16:P34">
+  <conditionalFormatting sqref="O4:P13 P14:P15 O16:P34 A4:M34">
     <cfRule type="expression" dxfId="104" priority="3">
       <formula>WEEKDAY($A4,2)=6</formula>
     </cfRule>
@@ -39328,9 +39589,9 @@
   </sheetPr>
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -39458,10 +39719,18 @@
         <f t="shared" ref="C4:C31" si="1">IF(ISERROR(VLOOKUP(B4,Feiertage,2,0)),"",(VLOOKUP(B4,Feiertage,2,0)))</f>
         <v>Pfingstmontag</v>
       </c>
-      <c r="D4" s="187"/>
-      <c r="E4" s="187"/>
-      <c r="F4" s="187"/>
-      <c r="G4" s="187"/>
+      <c r="D4" s="187">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E4" s="187">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="187">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G4" s="187">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="H4" s="188"/>
       <c r="I4" s="189" t="str">
         <f t="shared" ref="I4:I34" si="2">IF(A4="","",IF(G4=0,IF(K4=0,"",IF(PauseGTime&lt;IF(E4&gt;D4,E4-D4,1-D4+E4),IF(H4&lt;PauseGWert,"!",""),IF(PauseKTime&lt;IF(E4&gt;D4,E4-D4,1-D4+E4),IF(H4&lt;PauseKWert,"!",""),""))),IF(PauseGTime&lt;IF(G4&gt;D4,G4-D4,1-D4+G4),IF(IF(F4&gt;E4,F4-E4,1-E4+F4)+H4+0.0000001&lt;PauseGWert,"!",""),IF(PauseKTime&lt;IF(G4&gt;D4,G4-D4,1-D4+G4),IF(IF(F4&gt;E4,F4-E4,1-E4+F4)+H4+0.0000001&lt;PauseKWert,"!",""),""))))</f>
@@ -39470,7 +39739,7 @@
       <c r="J4" s="190"/>
       <c r="K4" s="191">
         <f t="shared" ref="K4:K34" si="3">IF(A4="","",IF(IF(D4&lt;E4,E4-D4,IF(E4="",0,E4-D4+1))+IF(F4&lt;G4,G4-F4,IF(G4="",0,G4-F4+1))-H4&gt;0,IF(D4&lt;E4,E4-D4,IF(E4="",0,E4-D4+1))+IF(F4&lt;G4,G4-F4,IF(G4="",0,G4-F4+1))-H4,0))</f>
-        <v>0</v>
+        <v>0.29166666666666657</v>
       </c>
       <c r="L4" s="192">
         <f t="shared" ref="L4:L34" ca="1" si="4">IF(AND(C4&lt;&gt;"",J4=""),IF(ISERROR(VLOOKUP(B4,Feiertage,2,0)),0,VLOOKUP(B4,Feiertage,3,0)*N4),IF(A4="",0,IF(J4&lt;&gt;"",IF(UPPER(J4)=VLOOKUP(UPPER(J4),Code,1,0),IF(OR(VLOOKUP(J4,Code,2,0)="NONE",VLOOKUP(J4,Code,2,0)="XTRA"),K4,IF(ISERROR(VLOOKUP(B4,Feiertage,2,0)),VLOOKUP(J4,Code,2,0)*N4,IF(VLOOKUP(B4,Feiertage,3,0)=0.5,IF(UPPER(J4)="G",VLOOKUP(B4,Feiertage,3,0)*VLOOKUP(J4,Code,2,0)*N4,0),VLOOKUP(B4,Feiertage,3,0)*VLOOKUP(J4,Code,2,0)*N4))),N4),N4)))</f>
@@ -39478,16 +39747,18 @@
       </c>
       <c r="M4" s="193">
         <f t="shared" ref="M4:M34" ca="1" si="5">IF(A4="","",ROUND(K4-L4,14))</f>
-        <v>0</v>
+        <v>0.29166666666667002</v>
       </c>
       <c r="N4" s="194">
         <f t="shared" ref="N4:N34" ca="1" si="6">IF(A4="","",INDIRECT(ADDRESS(MATCH(A4,SOLL_AZ_Ab,1)+11,WEEKDAY(A4,2)+3,,,"Voreinstellungen"),1))</f>
         <v>0</v>
       </c>
-      <c r="O4" s="195"/>
+      <c r="O4" s="195" t="s">
+        <v>174</v>
+      </c>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>1.83680555555556</v>
+        <v>3.0451388888888999</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39532,7 +39803,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>1.83680555555556</v>
+        <v>3.0451388888888999</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39548,11 +39819,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D6" s="200"/>
-      <c r="E6" s="200"/>
+      <c r="D6" s="200">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E6" s="200">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F6" s="200"/>
       <c r="G6" s="200"/>
-      <c r="H6" s="201"/>
+      <c r="H6" s="201">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I6" s="202" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -39560,7 +39837,7 @@
       <c r="J6" s="203"/>
       <c r="K6" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.35416666666666663</v>
       </c>
       <c r="L6" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -39568,16 +39845,18 @@
       </c>
       <c r="M6" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.33333333333332998</v>
+        <v>2.0833333333330002E-2</v>
       </c>
       <c r="N6" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0.33333333333333298</v>
       </c>
-      <c r="O6" s="208"/>
+      <c r="O6" s="208" t="s">
+        <v>173</v>
+      </c>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.5034722222222301</v>
+        <v>3.0659722222222299</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39593,19 +39872,25 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D7" s="200"/>
-      <c r="E7" s="200"/>
+      <c r="D7" s="200">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E7" s="200">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F7" s="200"/>
       <c r="G7" s="200"/>
-      <c r="H7" s="201"/>
+      <c r="H7" s="201">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="I7" s="202" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>!</v>
       </c>
       <c r="J7" s="203"/>
       <c r="K7" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.25694444444444436</v>
       </c>
       <c r="L7" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -39613,16 +39898,18 @@
       </c>
       <c r="M7" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.16666666666666999</v>
+        <v>9.0277777777779997E-2</v>
       </c>
       <c r="N7" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0.16666666666666699</v>
       </c>
-      <c r="O7" s="208"/>
+      <c r="O7" s="208" t="s">
+        <v>175</v>
+      </c>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.33680555555556</v>
+        <v>3.1562500000000102</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39638,19 +39925,25 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D8" s="200"/>
-      <c r="E8" s="200"/>
+      <c r="D8" s="200">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E8" s="200">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F8" s="200"/>
       <c r="G8" s="200"/>
-      <c r="H8" s="201"/>
+      <c r="H8" s="201">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="I8" s="202" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>!</v>
       </c>
       <c r="J8" s="203"/>
       <c r="K8" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.36111111111111105</v>
       </c>
       <c r="L8" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -39658,16 +39951,18 @@
       </c>
       <c r="M8" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.33333333333332998</v>
+        <v>2.777777777778E-2</v>
       </c>
       <c r="N8" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0.33333333333333298</v>
       </c>
-      <c r="O8" s="208"/>
+      <c r="O8" s="208" t="s">
+        <v>176</v>
+      </c>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0034722222222301</v>
+        <v>3.1840277777777901</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39712,7 +40007,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0034722222222301</v>
+        <v>3.1840277777777901</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39757,7 +40052,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0034722222222301</v>
+        <v>3.1840277777777901</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39802,7 +40097,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0034722222222301</v>
+        <v>3.1840277777777901</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39847,7 +40142,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0034722222222301</v>
+        <v>3.1840277777777901</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39892,7 +40187,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.67013888888890005</v>
+        <v>2.8506944444444602</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39937,7 +40232,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.50347222222222998</v>
+        <v>2.6840277777777901</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39982,7 +40277,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.1701388888889</v>
+        <v>2.3506944444444602</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40027,7 +40322,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.1701388888889</v>
+        <v>2.3506944444444602</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40072,7 +40367,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.1701388888889</v>
+        <v>2.3506944444444602</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40117,7 +40412,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.1701388888889</v>
+        <v>2.3506944444444602</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40162,7 +40457,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.1701388888889</v>
+        <v>2.3506944444444602</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40207,7 +40502,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.16319444444442999</v>
+        <v>2.0173611111111298</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40252,7 +40547,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3298611111111</v>
+        <v>1.85069444444446</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40297,7 +40592,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66319444444442999</v>
+        <v>1.51736111111113</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40342,7 +40637,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66319444444442999</v>
+        <v>1.51736111111113</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40387,7 +40682,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66319444444442999</v>
+        <v>1.51736111111113</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40432,7 +40727,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66319444444442999</v>
+        <v>1.51736111111113</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40477,7 +40772,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66319444444442999</v>
+        <v>1.51736111111113</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40522,7 +40817,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.99652777777776003</v>
+        <v>1.1840277777778001</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40567,7 +40862,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.16319444444443</v>
+        <v>1.01736111111113</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40612,7 +40907,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4965277777777599</v>
+        <v>0.68402777777779999</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40657,7 +40952,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4965277777777599</v>
+        <v>0.68402777777779999</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40702,7 +40997,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4965277777777599</v>
+        <v>0.68402777777779999</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40747,7 +41042,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4965277777777599</v>
+        <v>0.68402777777779999</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40792,7 +41087,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4965277777777599</v>
+        <v>0.68402777777779999</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40868,7 +41163,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">Mai!F40</f>
-        <v>1.83680555555556</v>
+        <v>2.7534722222222299</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -40933,7 +41228,7 @@
       </c>
       <c r="F38" s="246">
         <f>SUM(K4:K34)</f>
-        <v>0</v>
+        <v>1.2638888888888888</v>
       </c>
       <c r="G38" s="163"/>
       <c r="H38" s="163"/>
@@ -40989,14 +41284,14 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.4965277777777699</v>
+        <v>0.68402777777779</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
       <c r="I40" s="258"/>
       <c r="J40" s="259">
         <f>COUNTIF(K4:K34,"&gt;0")-IF(Voreinstellungen!C28="XTRA",COUNTIF(J4:J34,Voreinstellungen!B28),0)-IF(Voreinstellungen!C29="XTRA",COUNTIF(J4:J34,Voreinstellungen!B29),0)-IF(Voreinstellungen!C30="XTRA",COUNTIF(J4:J34,Voreinstellungen!B30),0)-IF(Voreinstellungen!C31="XTRA",COUNTIF(J4:J34,Voreinstellungen!B31),0)-IF(Voreinstellungen!C32="XTRA",COUNTIF(J4:J34,Voreinstellungen!B32),0)-IF(Voreinstellungen!C33="XTRA",COUNTIF(J4:J34,Voreinstellungen!B33),0)-COUNTIF(J4:J34,"H")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K40" s="382" t="s">
         <v>112</v>
@@ -41438,7 +41733,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.8298611111111001</v>
+        <v>0.35069444444446002</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41483,7 +41778,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.9965277777777699</v>
+        <v>0.18402777777779</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41528,7 +41823,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.3298611111111001</v>
+        <v>-0.14930555555554001</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41573,7 +41868,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.3298611111111001</v>
+        <v>-0.14930555555554001</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41618,7 +41913,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.3298611111111001</v>
+        <v>-0.14930555555554001</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41663,7 +41958,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.3298611111111001</v>
+        <v>-0.14930555555554001</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41708,7 +42003,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.3298611111111001</v>
+        <v>-0.14930555555554001</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41753,7 +42048,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.66319444444443</v>
+        <v>-0.48263888888887002</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41798,7 +42093,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.8298611111111001</v>
+        <v>-0.64930555555554004</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41843,7 +42138,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.16319444444443</v>
+        <v>-0.98263888888886997</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41888,7 +42183,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.16319444444443</v>
+        <v>-0.98263888888886997</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41933,7 +42228,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.16319444444443</v>
+        <v>-0.98263888888886997</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41978,7 +42273,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.16319444444443</v>
+        <v>-0.98263888888886997</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42023,7 +42318,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.16319444444443</v>
+        <v>-0.98263888888886997</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42068,7 +42363,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.4965277777777599</v>
+        <v>-1.3159722222221999</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42113,7 +42408,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.66319444444443</v>
+        <v>-1.48263888888887</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42158,7 +42453,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.9965277777777599</v>
+        <v>-1.8159722222221999</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42203,7 +42498,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.9965277777777599</v>
+        <v>-1.8159722222221999</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42248,7 +42543,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.9965277777777599</v>
+        <v>-1.8159722222221999</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42293,7 +42588,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.9965277777777599</v>
+        <v>-1.8159722222221999</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42338,7 +42633,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.9965277777777599</v>
+        <v>-1.8159722222221999</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42383,7 +42678,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.3298611111110903</v>
+        <v>-2.14930555555553</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42428,7 +42723,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.4965277777777599</v>
+        <v>-2.3159722222222001</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42473,7 +42768,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.8298611111110903</v>
+        <v>-2.64930555555553</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42518,7 +42813,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.8298611111110903</v>
+        <v>-2.64930555555553</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42563,7 +42858,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.8298611111110903</v>
+        <v>-2.64930555555553</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42608,7 +42903,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.8298611111110903</v>
+        <v>-2.64930555555553</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42653,7 +42948,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.8298611111110903</v>
+        <v>-2.64930555555553</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42698,7 +42993,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.1631944444444198</v>
+        <v>-2.98263888888886</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42743,7 +43038,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.3298611111110903</v>
+        <v>-3.14930555555553</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42788,7 +43083,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.6631944444444198</v>
+        <v>-3.48263888888886</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -42819,7 +43114,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">Juni!F40</f>
-        <v>-1.4965277777777699</v>
+        <v>0.68402777777779</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -42940,7 +43235,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-5.6631944444444304</v>
+        <v>-3.48263888888888</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>

</xml_diff>

<commit_message>
Tons of new info
</commit_message>
<xml_diff>
--- a/Admin/Arbeitszeiterfassung-2020-jcr.xlsx
+++ b/Admin/Arbeitszeiterfassung-2020-jcr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Projektarbeit_Docs\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5A327E-6971-4951-B45A-D8FB2897102F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D6B962-5B21-4E57-B5C1-43F4E66B50B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Voreinstellungen" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="186">
   <si>
     <t>Benutzer-Voreinstellungen</t>
   </si>
@@ -695,6 +695,18 @@
   </si>
   <si>
     <t>Results: Leds multichannel diff timers and matching the physical board</t>
+  </si>
+  <si>
+    <t>No Restuls: Lots of documentation about ecat and soes</t>
+  </si>
+  <si>
+    <t>Resultis: Soldering of pcb</t>
+  </si>
+  <si>
+    <t>Results: The connectors</t>
+  </si>
+  <si>
+    <t>Results: The SPI and programming was successfully tested on the PCB</t>
   </si>
 </sst>
 </file>
@@ -7401,6 +7413,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46C56183-4627-431E-8022-AEBD42E6F8A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE41107B-BC68-4C55-82FF-D549FA0D8CBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8625,6 +8745,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7836080F-D568-44A6-AC44-7CEE90B56F9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81A73BD1-894C-4886-A81F-783E00E4A38F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9590,7 +9818,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.8145833333333301</v>
+        <v>-0.56458333333333</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9635,7 +9863,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.8145833333333301</v>
+        <v>-0.56458333333333</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9680,7 +9908,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.8145833333333301</v>
+        <v>-0.56458333333333</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9725,7 +9953,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.8145833333333301</v>
+        <v>-0.56458333333333</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9770,7 +9998,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.14791666666666</v>
+        <v>-0.89791666666666003</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9815,7 +10043,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.3145833333333301</v>
+        <v>-1.0645833333333301</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9860,7 +10088,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.64791666666666</v>
+        <v>-1.39791666666666</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9905,7 +10133,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.64791666666666</v>
+        <v>-1.39791666666666</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9950,7 +10178,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.64791666666666</v>
+        <v>-1.39791666666666</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9995,7 +10223,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.64791666666666</v>
+        <v>-1.39791666666666</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10040,7 +10268,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.64791666666666</v>
+        <v>-1.39791666666666</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10085,7 +10313,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.98124999999999</v>
+        <v>-1.73124999999999</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10130,7 +10358,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.14791666666666</v>
+        <v>-1.89791666666666</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10175,7 +10403,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.48124999999999</v>
+        <v>-2.23124999999999</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10220,7 +10448,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.48124999999999</v>
+        <v>-2.23124999999999</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10265,7 +10493,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.48124999999999</v>
+        <v>-2.23124999999999</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10310,7 +10538,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.48124999999999</v>
+        <v>-2.23124999999999</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10355,7 +10583,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.48124999999999</v>
+        <v>-2.23124999999999</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10400,7 +10628,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.8145833333333199</v>
+        <v>-2.5645833333333199</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10445,7 +10673,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.98124999999999</v>
+        <v>-2.73124999999999</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10490,7 +10718,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.3145833333333199</v>
+        <v>-3.0645833333333199</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10535,7 +10763,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.3145833333333199</v>
+        <v>-3.0645833333333199</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10580,7 +10808,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.3145833333333199</v>
+        <v>-3.0645833333333199</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10625,7 +10853,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.3145833333333199</v>
+        <v>-3.0645833333333199</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10670,7 +10898,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.3145833333333199</v>
+        <v>-3.0645833333333199</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10715,7 +10943,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.6479166666666503</v>
+        <v>-3.3979166666666498</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10760,7 +10988,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.8145833333333199</v>
+        <v>-3.5645833333333199</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10805,7 +11033,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.1479166666666503</v>
+        <v>-3.8979166666666498</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10850,7 +11078,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.1479166666666503</v>
+        <v>-3.8979166666666498</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10895,7 +11123,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.1479166666666503</v>
+        <v>-3.8979166666666498</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10940,7 +11168,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.1479166666666503</v>
+        <v>-3.8979166666666498</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -10971,7 +11199,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">Juli!F40</f>
-        <v>-1.8145833333333301</v>
+        <v>-0.56458333333333</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -11092,7 +11320,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-5.14791666666666</v>
+        <v>-3.89791666666666</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -11541,7 +11769,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-5.14791666666666</v>
+        <v>-3.89791666666666</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11586,7 +11814,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-5.4812499999999904</v>
+        <v>-4.2312499999999904</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11631,7 +11859,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.64791666666666</v>
+        <v>-4.39791666666666</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11676,7 +11904,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.9812499999999904</v>
+        <v>-4.7312499999999904</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11721,7 +11949,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.9812499999999904</v>
+        <v>-4.7312499999999904</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11766,7 +11994,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.9812499999999904</v>
+        <v>-4.7312499999999904</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11811,7 +12039,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.9812499999999904</v>
+        <v>-4.7312499999999904</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11856,7 +12084,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.9812499999999904</v>
+        <v>-4.7312499999999904</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11901,7 +12129,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.3145833333333199</v>
+        <v>-5.0645833333333199</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11946,7 +12174,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.4812499999999904</v>
+        <v>-5.2312499999999904</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11991,7 +12219,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.8145833333333199</v>
+        <v>-5.5645833333333199</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12036,7 +12264,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.8145833333333199</v>
+        <v>-5.5645833333333199</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12081,7 +12309,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.8145833333333199</v>
+        <v>-5.5645833333333199</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12126,7 +12354,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.8145833333333199</v>
+        <v>-5.5645833333333199</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12171,7 +12399,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-6.8145833333333199</v>
+        <v>-5.5645833333333199</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12216,7 +12444,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.1479166666666503</v>
+        <v>-5.8979166666666503</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12261,7 +12489,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.3145833333333199</v>
+        <v>-6.0645833333333199</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12306,7 +12534,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.6479166666666503</v>
+        <v>-6.3979166666666503</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12351,7 +12579,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.6479166666666503</v>
+        <v>-6.3979166666666503</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12396,7 +12624,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.6479166666666503</v>
+        <v>-6.3979166666666503</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12441,7 +12669,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.6479166666666503</v>
+        <v>-6.3979166666666503</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12486,7 +12714,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.6479166666666503</v>
+        <v>-6.3979166666666503</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12531,7 +12759,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.9812499999999797</v>
+        <v>-6.7312499999999797</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12576,7 +12804,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.1479166666666494</v>
+        <v>-6.8979166666666503</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12621,7 +12849,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.4812499999999797</v>
+        <v>-7.2312499999999797</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12666,7 +12894,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.4812499999999797</v>
+        <v>-7.2312499999999797</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12711,7 +12939,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.4812499999999797</v>
+        <v>-7.2312499999999797</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12756,7 +12984,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.4812499999999797</v>
+        <v>-7.2312499999999797</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12801,7 +13029,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.4812499999999797</v>
+        <v>-7.2312499999999797</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12846,7 +13074,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-8.8145833333333101</v>
+        <v>-7.5645833333333101</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12922,7 +13150,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">August!F40</f>
-        <v>-5.14791666666666</v>
+        <v>-3.89791666666666</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -13043,7 +13271,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-8.8145833333333208</v>
+        <v>-7.5645833333333297</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -13492,7 +13720,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-8.9812499999999904</v>
+        <v>-7.7312500000000002</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13537,7 +13765,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-9.3145833333333208</v>
+        <v>-8.0645833333333297</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13582,7 +13810,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.3145833333333208</v>
+        <v>-8.0645833333333297</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13627,7 +13855,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.3145833333333208</v>
+        <v>-8.0645833333333297</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13672,7 +13900,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.3145833333333208</v>
+        <v>-8.0645833333333297</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13717,7 +13945,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.3145833333333208</v>
+        <v>-8.0645833333333297</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13762,7 +13990,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.6479166666666494</v>
+        <v>-8.39791666666666</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13807,7 +14035,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.8145833333333208</v>
+        <v>-8.5645833333333297</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13852,7 +14080,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.147916666666699</v>
+        <v>-8.89791666666666</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13897,7 +14125,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.147916666666699</v>
+        <v>-8.89791666666666</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13942,7 +14170,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.147916666666699</v>
+        <v>-8.89791666666666</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13987,7 +14215,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.147916666666699</v>
+        <v>-8.89791666666666</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14032,7 +14260,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.147916666666699</v>
+        <v>-8.89791666666666</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14077,7 +14305,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.481249999999999</v>
+        <v>-9.2312499999999904</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14122,7 +14350,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.647916666666699</v>
+        <v>-9.39791666666666</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14167,7 +14395,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.981249999999999</v>
+        <v>-9.7312499999999904</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14212,7 +14440,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.981249999999999</v>
+        <v>-9.7312499999999904</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14257,7 +14485,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.981249999999999</v>
+        <v>-9.7312499999999904</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14302,7 +14530,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.981249999999999</v>
+        <v>-9.7312499999999904</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14347,7 +14575,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-10.981249999999999</v>
+        <v>-9.7312499999999904</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14392,7 +14620,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.314583333333299</v>
+        <v>-10.064583333333299</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14437,7 +14665,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.481249999999999</v>
+        <v>-10.231249999999999</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14482,7 +14710,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.814583333333299</v>
+        <v>-10.564583333333299</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14527,7 +14755,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.814583333333299</v>
+        <v>-10.564583333333299</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14572,7 +14800,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.814583333333299</v>
+        <v>-10.564583333333299</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14617,7 +14845,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.814583333333299</v>
+        <v>-10.564583333333299</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14662,7 +14890,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-11.814583333333299</v>
+        <v>-10.564583333333299</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14707,7 +14935,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.1479166666666</v>
+        <v>-10.8979166666666</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14752,7 +14980,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.314583333333299</v>
+        <v>-11.064583333333299</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14797,7 +15025,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.6479166666666</v>
+        <v>-11.3979166666666</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14842,7 +15070,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.6479166666666</v>
+        <v>-11.3979166666666</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -14873,7 +15101,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">September!F40</f>
-        <v>-8.8145833333333208</v>
+        <v>-7.5645833333333297</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -14994,7 +15222,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-12.647916666666699</v>
+        <v>-11.397916666666699</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -15443,7 +15671,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-12.647916666666699</v>
+        <v>-11.397916666666699</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15488,7 +15716,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-12.647916666666699</v>
+        <v>-11.397916666666699</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15533,7 +15761,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.647916666666699</v>
+        <v>-11.397916666666699</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15578,7 +15806,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-12.981249999999999</v>
+        <v>-11.731249999999999</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15623,7 +15851,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.147916666666699</v>
+        <v>-11.897916666666699</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15668,7 +15896,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.481249999999999</v>
+        <v>-12.231249999999999</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15713,7 +15941,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.481249999999999</v>
+        <v>-12.231249999999999</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15758,7 +15986,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.481249999999999</v>
+        <v>-12.231249999999999</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15803,7 +16031,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.481249999999999</v>
+        <v>-12.231249999999999</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15848,7 +16076,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.481249999999999</v>
+        <v>-12.231249999999999</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15893,7 +16121,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.814583333333299</v>
+        <v>-12.564583333333299</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15938,7 +16166,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.981249999999999</v>
+        <v>-12.731249999999999</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15983,7 +16211,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.314583333333299</v>
+        <v>-13.064583333333299</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16028,7 +16256,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.314583333333299</v>
+        <v>-13.064583333333299</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16073,7 +16301,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.314583333333299</v>
+        <v>-13.064583333333299</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16118,7 +16346,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.314583333333299</v>
+        <v>-13.064583333333299</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16163,7 +16391,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.314583333333299</v>
+        <v>-13.064583333333299</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16208,7 +16436,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.6479166666666</v>
+        <v>-13.3979166666666</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16253,7 +16481,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-14.814583333333299</v>
+        <v>-13.564583333333299</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16298,7 +16526,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.1479166666666</v>
+        <v>-13.8979166666666</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16343,7 +16571,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.1479166666666</v>
+        <v>-13.8979166666666</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16388,7 +16616,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.1479166666666</v>
+        <v>-13.8979166666666</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16433,7 +16661,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.1479166666666</v>
+        <v>-13.8979166666666</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16478,7 +16706,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.1479166666666</v>
+        <v>-13.8979166666666</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16523,7 +16751,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.4812499999999</v>
+        <v>-14.2312499999999</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16568,7 +16796,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.6479166666666</v>
+        <v>-14.3979166666666</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16613,7 +16841,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.9812499999999</v>
+        <v>-14.7312499999999</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16658,7 +16886,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.9812499999999</v>
+        <v>-14.7312499999999</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16703,7 +16931,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.9812499999999</v>
+        <v>-14.7312499999999</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16748,7 +16976,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-15.9812499999999</v>
+        <v>-14.7312499999999</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16824,7 +17052,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">Oktober!F40</f>
-        <v>-12.647916666666699</v>
+        <v>-11.397916666666699</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -16945,7 +17173,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-15.981249999999999</v>
+        <v>-14.731249999999999</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -17394,7 +17622,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-15.981249999999999</v>
+        <v>-14.731249999999999</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17439,7 +17667,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-16.314583333333299</v>
+        <v>-15.064583333333299</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17484,7 +17712,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.481249999999999</v>
+        <v>-15.231249999999999</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17529,7 +17757,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.814583333333299</v>
+        <v>-15.564583333333299</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17574,7 +17802,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.814583333333299</v>
+        <v>-15.564583333333299</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17619,7 +17847,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.814583333333299</v>
+        <v>-15.564583333333299</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17664,7 +17892,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.814583333333299</v>
+        <v>-15.564583333333299</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17709,7 +17937,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-16.814583333333299</v>
+        <v>-15.564583333333299</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17754,7 +17982,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.1479166666666</v>
+        <v>-15.8979166666666</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17799,7 +18027,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.314583333333299</v>
+        <v>-16.064583333333299</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17844,7 +18072,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.6479166666666</v>
+        <v>-16.3979166666666</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17889,7 +18117,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.6479166666666</v>
+        <v>-16.3979166666666</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17934,7 +18162,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.6479166666666</v>
+        <v>-16.3979166666666</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17979,7 +18207,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.6479166666666</v>
+        <v>-16.3979166666666</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18024,7 +18252,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.6479166666666</v>
+        <v>-16.3979166666666</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18069,7 +18297,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-17.9812499999999</v>
+        <v>-16.7312499999999</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18114,7 +18342,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.1479166666666</v>
+        <v>-16.8979166666666</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18159,7 +18387,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.4812499999999</v>
+        <v>-17.2312499999999</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18204,7 +18432,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.4812499999999</v>
+        <v>-17.2312499999999</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18249,7 +18477,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.4812499999999</v>
+        <v>-17.2312499999999</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18294,7 +18522,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.4812499999999</v>
+        <v>-17.2312499999999</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18339,7 +18567,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.4812499999999</v>
+        <v>-17.2312499999999</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18384,7 +18612,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.8145833333332</v>
+        <v>-17.5645833333332</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18429,7 +18657,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.8979166666665</v>
+        <v>-17.6479166666665</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18474,7 +18702,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.8979166666665</v>
+        <v>-17.6479166666665</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18519,7 +18747,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.8979166666665</v>
+        <v>-17.6479166666665</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18564,7 +18792,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.8979166666665</v>
+        <v>-17.6479166666665</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18609,7 +18837,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.8979166666665</v>
+        <v>-17.6479166666665</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18654,7 +18882,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-18.8979166666665</v>
+        <v>-17.6479166666665</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18699,7 +18927,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.2312499999998</v>
+        <v>-17.9812499999998</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -18744,7 +18972,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-19.314583333333101</v>
+        <v>-18.064583333333101</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -18775,7 +19003,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">November!F40</f>
-        <v>-15.981249999999999</v>
+        <v>-14.731249999999999</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -18896,7 +19124,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-19.314583333333299</v>
+        <v>-18.064583333333299</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
@@ -22183,9 +22411,9 @@
         <f>Juni!A22</f>
         <v>42539</v>
       </c>
-      <c r="R22" s="294" t="str">
+      <c r="R22" s="294">
         <f>IF(Juni!K22&gt;0,Juni!K22,"")</f>
-        <v/>
+        <v>0.35416666666666674</v>
       </c>
       <c r="S22" s="299" t="str">
         <f>IF(OR(Juni!C22="",Juni!J22&lt;&gt;""),UPPER(Juni!J22),"F")</f>
@@ -22335,9 +22563,9 @@
         <f>Juni!A23</f>
         <v>42540</v>
       </c>
-      <c r="R23" s="294" t="str">
+      <c r="R23" s="294">
         <f>IF(Juni!K23&gt;0,Juni!K23,"")</f>
-        <v/>
+        <v>0.35416666666666663</v>
       </c>
       <c r="S23" s="299" t="str">
         <f>IF(OR(Juni!C23="",Juni!J23&lt;&gt;""),UPPER(Juni!J23),"F")</f>
@@ -22487,9 +22715,9 @@
         <f>Juni!A24</f>
         <v>42541</v>
       </c>
-      <c r="R24" s="294" t="str">
+      <c r="R24" s="294">
         <f>IF(Juni!K24&gt;0,Juni!K24,"")</f>
-        <v/>
+        <v>0.16666666666666663</v>
       </c>
       <c r="S24" s="299" t="str">
         <f>IF(OR(Juni!C24="",Juni!J24&lt;&gt;""),UPPER(Juni!J24),"F")</f>
@@ -22943,9 +23171,9 @@
         <f>Juni!A27</f>
         <v>42544</v>
       </c>
-      <c r="R27" s="294" t="str">
+      <c r="R27" s="294">
         <f>IF(Juni!K27&gt;0,Juni!K27,"")</f>
-        <v/>
+        <v>0.375</v>
       </c>
       <c r="S27" s="299" t="str">
         <f>IF(OR(Juni!C27="",Juni!J27&lt;&gt;""),UPPER(Juni!J27),"F")</f>
@@ -24208,7 +24436,7 @@
       <c r="P36" s="318"/>
       <c r="Q36" s="398">
         <f>Juni!F38</f>
-        <v>2.931944444444444</v>
+        <v>4.1819444444444436</v>
       </c>
       <c r="R36" s="398"/>
       <c r="S36" s="317"/>
@@ -24250,7 +24478,7 @@
       <c r="AK36" s="317"/>
       <c r="AL36" s="319">
         <f t="shared" si="0"/>
-        <v>12.352083333333336</v>
+        <v>13.602083333333336</v>
       </c>
     </row>
     <row r="37" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -24289,7 +24517,7 @@
       <c r="P37" s="323"/>
       <c r="Q37" s="393">
         <f ca="1">ROUND(Q36-Q35,10)</f>
-        <v>-0.40138888890000002</v>
+        <v>0.84861111109999998</v>
       </c>
       <c r="R37" s="393"/>
       <c r="S37" s="322"/>
@@ -24331,7 +24559,7 @@
       <c r="AK37" s="322"/>
       <c r="AL37" s="324">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.3145833333</v>
+        <v>-18.0645833333</v>
       </c>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.25">
@@ -24370,7 +24598,7 @@
       <c r="P38" s="395"/>
       <c r="Q38" s="395">
         <f>Juni!J40</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="R38" s="395"/>
       <c r="S38" s="395"/>
@@ -24412,7 +24640,7 @@
       <c r="AK38" s="395"/>
       <c r="AL38" s="326">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
@@ -29189,7 +29417,7 @@
       <c r="C2" s="346"/>
       <c r="D2" s="347">
         <f>Jahresübersicht!AL38</f>
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="79" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
@@ -29210,7 +29438,7 @@
       <c r="C4" s="346"/>
       <c r="D4" s="349">
         <f>D2*D3</f>
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="79" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
@@ -29237,7 +29465,7 @@
       <c r="C6" s="354"/>
       <c r="D6" s="355">
         <f>D5*D2</f>
-        <v>9.6</v>
+        <v>10.799999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="79" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
@@ -33651,7 +33879,7 @@
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -35618,7 +35846,7 @@
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
@@ -37731,8 +37959,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
@@ -39820,9 +40048,9 @@
   </sheetPr>
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -40834,11 +41062,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D22" s="200"/>
-      <c r="E22" s="200"/>
+      <c r="D22" s="200">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E22" s="200">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="F22" s="200"/>
       <c r="G22" s="200"/>
-      <c r="H22" s="201"/>
+      <c r="H22" s="201">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I22" s="202" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -40846,7 +41080,7 @@
       <c r="J22" s="203"/>
       <c r="K22" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.35416666666666674</v>
       </c>
       <c r="L22" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -40854,16 +41088,18 @@
       </c>
       <c r="M22" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.33333333333332998</v>
+        <v>2.0833333333330002E-2</v>
       </c>
       <c r="N22" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0.33333333333333298</v>
       </c>
-      <c r="O22" s="208"/>
+      <c r="O22" s="208" t="s">
+        <v>182</v>
+      </c>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>3.1854166666666899</v>
+        <v>3.5395833333333502</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40879,11 +41115,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D23" s="200"/>
-      <c r="E23" s="200"/>
+      <c r="D23" s="200">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E23" s="200">
+        <v>0.9375</v>
+      </c>
       <c r="F23" s="200"/>
       <c r="G23" s="200"/>
-      <c r="H23" s="201"/>
+      <c r="H23" s="201">
+        <v>6.25E-2</v>
+      </c>
       <c r="I23" s="202" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -40891,7 +41133,7 @@
       <c r="J23" s="203"/>
       <c r="K23" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.35416666666666663</v>
       </c>
       <c r="L23" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -40899,16 +41141,18 @@
       </c>
       <c r="M23" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>0.35416666666667002</v>
       </c>
       <c r="N23" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="O23" s="208"/>
+      <c r="O23" s="208" t="s">
+        <v>183</v>
+      </c>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>3.1854166666666899</v>
+        <v>3.8937500000000198</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40924,8 +41168,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D24" s="200"/>
-      <c r="E24" s="200"/>
+      <c r="D24" s="200">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E24" s="200">
+        <v>0.875</v>
+      </c>
       <c r="F24" s="200"/>
       <c r="G24" s="200"/>
       <c r="H24" s="201"/>
@@ -40936,7 +41184,7 @@
       <c r="J24" s="203"/>
       <c r="K24" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="L24" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -40944,16 +41192,18 @@
       </c>
       <c r="M24" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>0.16666666666666999</v>
       </c>
       <c r="N24" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="O24" s="208"/>
+      <c r="O24" s="208" t="s">
+        <v>184</v>
+      </c>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>3.1854166666666899</v>
+        <v>4.0604166666666899</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40998,7 +41248,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>3.1854166666666899</v>
+        <v>4.0604166666666899</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41043,7 +41293,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>3.1854166666666899</v>
+        <v>4.0604166666666899</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41059,19 +41309,25 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D27" s="200"/>
-      <c r="E27" s="200"/>
+      <c r="D27" s="200">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E27" s="200">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F27" s="200"/>
       <c r="G27" s="200"/>
-      <c r="H27" s="201"/>
+      <c r="H27" s="201">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I27" s="202" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>!</v>
       </c>
       <c r="J27" s="203"/>
       <c r="K27" s="204">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="L27" s="205">
         <f t="shared" ca="1" si="4"/>
@@ -41079,16 +41335,18 @@
       </c>
       <c r="M27" s="206">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.33333333333332998</v>
+        <v>4.1666666666670002E-2</v>
       </c>
       <c r="N27" s="207">
         <f t="shared" ca="1" si="6"/>
         <v>0.33333333333333298</v>
       </c>
-      <c r="O27" s="208"/>
+      <c r="O27" s="208" t="s">
+        <v>185</v>
+      </c>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8520833333333599</v>
+        <v>4.1020833333333604</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41133,7 +41391,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>2.6854166666666899</v>
+        <v>3.9354166666666899</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41178,7 +41436,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>2.3520833333333599</v>
+        <v>3.6020833333333599</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41223,7 +41481,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>2.3520833333333599</v>
+        <v>3.6020833333333599</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41268,7 +41526,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>2.3520833333333599</v>
+        <v>3.6020833333333599</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41313,7 +41571,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>2.3520833333333599</v>
+        <v>3.6020833333333599</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41358,7 +41616,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>2.3520833333333599</v>
+        <v>3.6020833333333599</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -41499,7 +41757,7 @@
       </c>
       <c r="F38" s="246">
         <f>SUM(K4:K34)</f>
-        <v>2.931944444444444</v>
+        <v>4.1819444444444436</v>
       </c>
       <c r="G38" s="163"/>
       <c r="H38" s="163"/>
@@ -41555,14 +41813,14 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>2.35208333333334</v>
+        <v>3.60208333333334</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>
       <c r="I40" s="258"/>
       <c r="J40" s="259">
         <f>COUNTIF(K4:K34,"&gt;0")-IF(Voreinstellungen!C28="XTRA",COUNTIF(J4:J34,Voreinstellungen!B28),0)-IF(Voreinstellungen!C29="XTRA",COUNTIF(J4:J34,Voreinstellungen!B29),0)-IF(Voreinstellungen!C30="XTRA",COUNTIF(J4:J34,Voreinstellungen!B30),0)-IF(Voreinstellungen!C31="XTRA",COUNTIF(J4:J34,Voreinstellungen!B31),0)-IF(Voreinstellungen!C32="XTRA",COUNTIF(J4:J34,Voreinstellungen!B32),0)-IF(Voreinstellungen!C33="XTRA",COUNTIF(J4:J34,Voreinstellungen!B33),0)-COUNTIF(J4:J34,"H")</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K40" s="382" t="s">
         <v>112</v>
@@ -42004,7 +42262,7 @@
       <c r="O4" s="195"/>
       <c r="P4" s="196">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>2.01875000000001</v>
+        <v>3.26875000000001</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42049,7 +42307,7 @@
       <c r="O5" s="208"/>
       <c r="P5" s="209">
         <f t="shared" ref="P5:P34" ca="1" si="8">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>1.85208333333334</v>
+        <v>3.10208333333334</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42094,7 +42352,7 @@
       <c r="O6" s="208"/>
       <c r="P6" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.51875000000001</v>
+        <v>2.76875000000001</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42139,7 +42397,7 @@
       <c r="O7" s="208"/>
       <c r="P7" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.51875000000001</v>
+        <v>2.76875000000001</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42184,7 +42442,7 @@
       <c r="O8" s="208"/>
       <c r="P8" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.51875000000001</v>
+        <v>2.76875000000001</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42229,7 +42487,7 @@
       <c r="O9" s="208"/>
       <c r="P9" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.51875000000001</v>
+        <v>2.76875000000001</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42274,7 +42532,7 @@
       <c r="O10" s="208"/>
       <c r="P10" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.51875000000001</v>
+        <v>2.76875000000001</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42319,7 +42577,7 @@
       <c r="O11" s="208"/>
       <c r="P11" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.1854166666666801</v>
+        <v>2.4354166666666801</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42364,7 +42622,7 @@
       <c r="O12" s="208"/>
       <c r="P12" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>1.01875000000001</v>
+        <v>2.26875000000001</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42409,7 +42667,7 @@
       <c r="O13" s="208"/>
       <c r="P13" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.68541666666668</v>
+        <v>1.9354166666666801</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42454,7 +42712,7 @@
       <c r="O14" s="208"/>
       <c r="P14" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.68541666666668</v>
+        <v>1.9354166666666801</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42499,7 +42757,7 @@
       <c r="O15" s="208"/>
       <c r="P15" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.68541666666668</v>
+        <v>1.9354166666666801</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42544,7 +42802,7 @@
       <c r="O16" s="208"/>
       <c r="P16" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.68541666666668</v>
+        <v>1.9354166666666801</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42589,7 +42847,7 @@
       <c r="O17" s="208"/>
       <c r="P17" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.68541666666668</v>
+        <v>1.9354166666666801</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42634,7 +42892,7 @@
       <c r="O18" s="208"/>
       <c r="P18" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.35208333333335001</v>
+        <v>1.60208333333335</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42679,7 +42937,7 @@
       <c r="O19" s="208"/>
       <c r="P19" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>0.18541666666668</v>
+        <v>1.4354166666666801</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42724,7 +42982,7 @@
       <c r="O20" s="208"/>
       <c r="P20" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.14791666666664999</v>
+        <v>1.10208333333335</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42769,7 +43027,7 @@
       <c r="O21" s="208"/>
       <c r="P21" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.14791666666664999</v>
+        <v>1.10208333333335</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42814,7 +43072,7 @@
       <c r="O22" s="208"/>
       <c r="P22" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.14791666666664999</v>
+        <v>1.10208333333335</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42859,7 +43117,7 @@
       <c r="O23" s="208"/>
       <c r="P23" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.14791666666664999</v>
+        <v>1.10208333333335</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42904,7 +43162,7 @@
       <c r="O24" s="208"/>
       <c r="P24" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.14791666666664999</v>
+        <v>1.10208333333335</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42949,7 +43207,7 @@
       <c r="O25" s="208"/>
       <c r="P25" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.48124999999998003</v>
+        <v>0.76875000000002003</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -42994,7 +43252,7 @@
       <c r="O26" s="208"/>
       <c r="P26" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.64791666666665004</v>
+        <v>0.60208333333334996</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -43039,7 +43297,7 @@
       <c r="O27" s="208"/>
       <c r="P27" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.98124999999997997</v>
+        <v>0.26875000000001997</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -43084,7 +43342,7 @@
       <c r="O28" s="208"/>
       <c r="P28" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.98124999999997997</v>
+        <v>0.26875000000001997</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -43129,7 +43387,7 @@
       <c r="O29" s="208"/>
       <c r="P29" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.98124999999997997</v>
+        <v>0.26875000000001997</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -43174,7 +43432,7 @@
       <c r="O30" s="208"/>
       <c r="P30" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.98124999999997997</v>
+        <v>0.26875000000001997</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -43219,7 +43477,7 @@
       <c r="O31" s="208"/>
       <c r="P31" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.98124999999997997</v>
+        <v>0.26875000000001997</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -43264,7 +43522,7 @@
       <c r="O32" s="208"/>
       <c r="P32" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.3145833333333099</v>
+        <v>-6.4583333333309997E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -43309,7 +43567,7 @@
       <c r="O33" s="208"/>
       <c r="P33" s="209">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.48124999999998</v>
+        <v>-0.23124999999998</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="89" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -43354,7 +43612,7 @@
       <c r="O34" s="221"/>
       <c r="P34" s="222">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.8145833333333099</v>
+        <v>-0.56458333333331001</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="89" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -43385,7 +43643,7 @@
       </c>
       <c r="F36" s="232">
         <f ca="1">Juni!F40</f>
-        <v>2.35208333333334</v>
+        <v>3.60208333333334</v>
       </c>
       <c r="G36" s="163"/>
       <c r="H36" s="163"/>
@@ -43506,7 +43764,7 @@
       </c>
       <c r="F40" s="257">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.8145833333333301</v>
+        <v>-0.56458333333333</v>
       </c>
       <c r="G40" s="163"/>
       <c r="H40" s="163"/>

</xml_diff>